<commit_message>
learn if, count if, count, average
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D57594B-838E-4614-B8AD-827E8D6BA406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0C52D5-2648-4AA9-91E6-9DE2EB30AF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
+    <sheet name="PHASE1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Day</t>
   </si>
@@ -541,13 +542,100 @@
       </rPr>
       <t xml:space="preserve"> with a user form, automated stock updates &amp; dashboard</t>
     </r>
+  </si>
+  <si>
+    <t>Practical Tasks (Beginner-Friendly)</t>
+  </si>
+  <si>
+    <t>1️⃣ Student Marksheet with Conditional Formatting (Main Practice Task)</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Quinn</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Tina</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Mean mark</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>COUNT OF STUDENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,8 +656,48 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +707,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -627,11 +761,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -943,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D52DEAC-DA9C-4AAE-B79E-917F758942A1}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1079,4 +1248,380 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB262F42-5A31-4E7C-9BC0-8AA576C134EE}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" ht="21">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="7" spans="1:13" ht="24">
+      <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3">
+        <v>78</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f>IF(C8&gt;=50,"PASS", "FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="F8" s="11">
+        <f>COUNT(C8:C27)</f>
+        <v>20</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11">
+        <f>AVERAGE(C8:C27)</f>
+        <v>69.3</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11">
+        <f>COUNTIF(D8:D27,"PASS")</f>
+        <v>16</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11">
+        <f>F8-J8</f>
+        <v>4</v>
+      </c>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3">
+        <v>55</v>
+      </c>
+      <c r="D9" s="9" t="str">
+        <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,"PASS", "FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3">
+        <v>90</v>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3">
+        <v>88</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="3">
+        <v>60</v>
+      </c>
+      <c r="D13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3">
+        <v>72</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3">
+        <v>34</v>
+      </c>
+      <c r="D15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3">
+        <v>95</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3">
+        <v>80</v>
+      </c>
+      <c r="D17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3">
+        <v>91</v>
+      </c>
+      <c r="D19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="3">
+        <v>62</v>
+      </c>
+      <c r="D20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3">
+        <v>87</v>
+      </c>
+      <c r="D21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3">
+        <v>39</v>
+      </c>
+      <c r="D22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3">
+        <v>76</v>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="3">
+        <v>59</v>
+      </c>
+      <c r="D24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="3">
+        <v>98</v>
+      </c>
+      <c r="D25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42</v>
+      </c>
+      <c r="D26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3">
+        <v>85</v>
+      </c>
+      <c r="D27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G10"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B4:H5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I10"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C8:C27">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improve countif, unique, ...
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0C52D5-2648-4AA9-91E6-9DE2EB30AF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865A8D9E-583C-41CC-AF3A-2473CFD2E39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
     <sheet name="PHASE1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PHASE1!$B$32:$D$52</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>Day</t>
   </si>
@@ -629,6 +654,72 @@
   </si>
   <si>
     <t>COUNT OF STUDENT</t>
+  </si>
+  <si>
+    <t>bool result</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>2️⃣ Sales Data Analysis (Sorting &amp; Filtering)</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>east</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>give the different type</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
   </si>
 </sst>
 </file>
@@ -697,7 +788,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +804,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -761,17 +864,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -779,17 +879,82 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1252,80 +1417,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB262F42-5A31-4E7C-9BC0-8AA576C134EE}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="24">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -1334,30 +1499,30 @@
       <c r="C8" s="3">
         <v>78</v>
       </c>
-      <c r="D8" s="9" t="str">
-        <f>IF(C8&gt;=50,"PASS", "FAIL")</f>
+      <c r="D8" s="7" t="str">
+        <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11">
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="11"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -1366,18 +1531,18 @@
       <c r="C9" s="3">
         <v>55</v>
       </c>
-      <c r="D9" s="9" t="str">
-        <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,"PASS", "FAIL")</f>
+      <c r="D9" s="7" t="str">
+        <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -1386,18 +1551,18 @@
       <c r="C10" s="3">
         <v>90</v>
       </c>
-      <c r="D10" s="9" t="str">
+      <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -1406,7 +1571,7 @@
       <c r="C11" s="3">
         <v>45</v>
       </c>
-      <c r="D11" s="9" t="str">
+      <c r="D11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
@@ -1418,7 +1583,7 @@
       <c r="C12" s="3">
         <v>88</v>
       </c>
-      <c r="D12" s="9" t="str">
+      <c r="D12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
@@ -1430,7 +1595,7 @@
       <c r="C13" s="3">
         <v>60</v>
       </c>
-      <c r="D13" s="9" t="str">
+      <c r="D13" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
@@ -1442,10 +1607,14 @@
       <c r="C14" s="3">
         <v>72</v>
       </c>
-      <c r="D14" s="9" t="str">
+      <c r="D14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
+      <c r="F14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="3" t="s">
@@ -1454,9 +1623,15 @@
       <c r="C15" s="3">
         <v>34</v>
       </c>
-      <c r="D15" s="9" t="str">
+      <c r="D15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1466,145 +1641,459 @@
       <c r="C16" s="3">
         <v>95</v>
       </c>
-      <c r="D16" s="9" t="str">
+      <c r="D16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:8">
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="3">
         <v>80</v>
       </c>
-      <c r="D17" s="9" t="str">
+      <c r="D17" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:8">
       <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="3">
         <v>50</v>
       </c>
-      <c r="D18" s="9" t="str">
+      <c r="D18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:8">
       <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="3">
         <v>91</v>
       </c>
-      <c r="D19" s="9" t="str">
+      <c r="D19" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:8">
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="3">
         <v>62</v>
       </c>
-      <c r="D20" s="9" t="str">
+      <c r="D20" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:8">
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="3">
         <v>87</v>
       </c>
-      <c r="D21" s="9" t="str">
+      <c r="D21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:8">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="3">
         <v>39</v>
       </c>
-      <c r="D22" s="9" t="str">
+      <c r="D22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:8">
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="3">
         <v>76</v>
       </c>
-      <c r="D23" s="9" t="str">
+      <c r="D23" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:8">
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="3">
         <v>59</v>
       </c>
-      <c r="D24" s="9" t="str">
+      <c r="D24" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:8">
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="3">
         <v>98</v>
       </c>
-      <c r="D25" s="9" t="str">
+      <c r="D25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:8">
       <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="3">
         <v>42</v>
       </c>
-      <c r="D26" s="9" t="str">
+      <c r="D26" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:8">
       <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="3">
         <v>85</v>
       </c>
-      <c r="D27" s="9" t="str">
+      <c r="D27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="19">
+        <v>900</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="19">
+        <v>850</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="J34" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K34" s="20"/>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="19">
+        <v>800</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="15">
+        <f>COUNTIF(D33:D52,F35)</f>
+        <v>6</v>
+      </c>
+      <c r="J35" s="22" t="str" cm="1">
+        <f t="array" ref="J35:J37">_xlfn.UNIQUE(B33:B52)</f>
+        <v>Tablet</v>
+      </c>
+      <c r="K35" s="15">
+        <f>COUNTIF(B33:B52,J35)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="19">
+        <v>780</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="15">
+        <f t="shared" ref="G36:G38" si="1">COUNTIF(D34:D53,F36)</f>
+        <v>5</v>
+      </c>
+      <c r="J36" s="22" t="str">
+        <v>Laptop</v>
+      </c>
+      <c r="K36" s="15">
+        <f t="shared" ref="K36:K37" si="2">COUNTIF(B34:B53,J36)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="19">
+        <v>750</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J37" s="22" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="19">
+        <v>700</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="19">
+        <v>700</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="19">
+        <v>640</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="19">
+        <v>620</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="19">
+        <v>600</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="19">
+        <v>550</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="19">
+        <v>530</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="19">
+        <v>520</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="19">
+        <v>500</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="19">
+        <v>500</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="19">
+        <v>480</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="19">
+        <v>450</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="19">
+        <v>410</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="19">
+        <v>400</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="19">
+        <v>300</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <autoFilter ref="B32:D52" xr:uid="{AB262F42-5A31-4E7C-9BC0-8AA576C134EE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:D52">
+    <sortCondition descending="1" ref="C33:C52"/>
+  </sortState>
+  <mergeCells count="14">
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="J34:K34"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M10"/>
     <mergeCell ref="F7:G7"/>
@@ -1617,8 +2106,20 @@
     <mergeCell ref="J7:K7"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C27">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D27">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add pivot table and pivot chart
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865A8D9E-583C-41CC-AF3A-2473CFD2E39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70985B33-8729-49D0-89D3-7397B4C9E6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,32 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PHASE1!$B$32:$D$52</definedName>
+    <definedName name="_xlcn.WorksheetConnection_PHASE1B32D52" hidden="1">PHASE1!$B$32:$D$52</definedName>
+    <definedName name="Slicer_Region">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="21" r:id="rId3"/>
+    <pivotCache cacheId="25" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId5"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Range" name="Range" connection="WorksheetConnection_PHASE1!$B$32:$D$52"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,6 +56,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{D1933D6D-99F8-46D5-8144-7DE80C111076}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="7" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" xr16:uid="{DBC9E555-51E4-4A29-BEFC-86E5DC350A6E}" name="WorksheetConnection_PHASE1!$B$32:$D$52" type="102" refreshedVersion="7" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Range" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_PHASE1B32D52"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
   <si>
     <t>Day</t>
   </si>
@@ -720,6 +764,21 @@
   </si>
   <si>
     <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Sales</t>
+  </si>
+  <si>
+    <t>Sum of Marks</t>
+  </si>
+  <si>
+    <t>&gt; using unique</t>
   </si>
 </sst>
 </file>
@@ -788,7 +847,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,6 +875,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +912,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,6 +938,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,32 +974,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="0"/>
@@ -922,36 +995,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -976,6 +1019,2381 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[time line.xlsx]PHASE1!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PHASE1!$N$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PHASE1!$M$35:$M$38</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Laptop</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Phone</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tablet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PHASE1!$N$35:$N$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7084-4259-84A2-29E07747BA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1347473535"/>
+        <c:axId val="1347474783"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1347473535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1347474783"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1347474783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1347473535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[time line.xlsx]PHASE1!PivotTable4</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PHASE1!$L$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>PHASE1!$K$14:$K$16</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>FAIL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PASS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PHASE1!$L$14:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE48-4906-98BD-85432C831090}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D373FC-6A76-4EF5-8EDA-FB3FA40FE4E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Region">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A93A7A-4F28-44F6-B1C3-EE92BC30ECC6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7840980" y="7322821"/>
+              <a:ext cx="1668780" cy="1645919"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDBFBFC-974C-4F40-8C16-82AA0EC6FE0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="raphael Randrianantoanina" refreshedDate="45737.655381712961" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="20" xr:uid="{F7A3B827-05DD-42B9-B07C-2B085B6D1543}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B32:D52" sheet="PHASE1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Tablet"/>
+        <s v="Laptop"/>
+        <s v="Phone"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="300" maxValue="900"/>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="4">
+        <s v="West"/>
+        <s v="North"/>
+        <s v="South"/>
+        <s v="East"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="8329306"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="raphael Randrianantoanina" refreshedDate="45737.657730092593" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="20" xr:uid="{24F6D42A-1A2A-4215-BD16-35DB4915FCDB}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B7:D27" sheet="PHASE1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Student Name" numFmtId="0">
+      <sharedItems count="20">
+        <s v="Alice"/>
+        <s v="Bob"/>
+        <s v="Charlie"/>
+        <s v="David"/>
+        <s v="Emma"/>
+        <s v="Frank"/>
+        <s v="Grace"/>
+        <s v="Henry"/>
+        <s v="Ivy"/>
+        <s v="Jack"/>
+        <s v="Kevin"/>
+        <s v="Lily"/>
+        <s v="Mike"/>
+        <s v="Nora"/>
+        <s v="Oliver"/>
+        <s v="Peter"/>
+        <s v="Quinn"/>
+        <s v="Rachel"/>
+        <s v="Steve"/>
+        <s v="Tina"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Marks" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="34" maxValue="98"/>
+    </cacheField>
+    <cacheField name="Result" numFmtId="0">
+      <sharedItems count="2">
+        <s v="PASS"/>
+        <s v="FAIL"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
+  <r>
+    <x v="0"/>
+    <n v="900"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="850"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="800"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="780"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="750"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="700"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="700"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="640"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="620"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="600"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="550"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="530"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="520"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="500"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="500"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="480"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="450"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="410"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="400"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="300"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
+  <r>
+    <x v="0"/>
+    <n v="78"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="55"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="90"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="45"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="88"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="60"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="72"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="34"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="95"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="80"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="50"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="91"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="62"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="87"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="39"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="76"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="59"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="98"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="42"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="85"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF3B0386-B4D1-4CF8-83F4-0817675386DD}" name="PivotTable4" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="K13:L16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Marks" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1DF83544-1957-4782-820D-0D69E5BDDAF3}" name="PivotTable3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="M34:N38" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item h="1" x="3"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Region" xr10:uid="{40F3485E-B352-41FB-8FC7-1B23E203BE9E}" sourceName="Region">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable3"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="8329306">
+      <items count="4">
+        <i x="3"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Region" xr10:uid="{7D7080CB-6C8B-4707-A1FD-87B70AE45869}" cache="Slicer_Region" caption="Region" rowHeight="234950"/>
+</slicers>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1417,53 +3835,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB262F42-5A31-4E7C-9BC0-8AA576C134EE}">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E30" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -1475,22 +3899,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="I7" s="18"/>
+      <c r="J7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="18"/>
+      <c r="L7" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -1503,26 +3927,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="19">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10">
+      <c r="G8" s="19"/>
+      <c r="H8" s="19">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10">
+      <c r="I8" s="19"/>
+      <c r="J8" s="19">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10">
+      <c r="K8" s="19"/>
+      <c r="L8" s="19">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -1535,14 +3959,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -1555,14 +3979,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -1599,6 +4023,12 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
+      <c r="K13" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="3" t="s">
@@ -1615,6 +4045,12 @@
         <v>64</v>
       </c>
       <c r="G14" s="14"/>
+      <c r="K14" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="25">
+        <v>160</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="3" t="s">
@@ -1627,11 +4063,17 @@
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="9" t="s">
         <v>66</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="25">
+        <v>1226</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1645,6 +4087,12 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
+      <c r="K16" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="25">
+        <v>1386</v>
+      </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="3" t="s">
@@ -1779,189 +4227,219 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:14">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="11">
         <v>900</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:14">
       <c r="B34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="11">
         <v>850</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="J34" s="20" t="s">
+      <c r="G34" s="17"/>
+      <c r="J34" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="20"/>
-    </row>
-    <row r="35" spans="2:11">
+      <c r="K34" s="17"/>
+      <c r="M34" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="N34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
       <c r="B35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="11">
         <v>800</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="9">
         <f>COUNTIF(D33:D52,F35)</f>
         <v>6</v>
       </c>
-      <c r="J35" s="22" t="str" cm="1">
+      <c r="J35" s="13" t="str" cm="1">
         <f t="array" ref="J35:J37">_xlfn.UNIQUE(B33:B52)</f>
         <v>Tablet</v>
       </c>
-      <c r="K35" s="15">
+      <c r="K35" s="9">
         <f>COUNTIF(B33:B52,J35)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="2:11">
+      <c r="M35" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="N35" s="25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
       <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="11">
         <v>780</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="9">
         <f t="shared" ref="G36:G38" si="1">COUNTIF(D34:D53,F36)</f>
         <v>5</v>
       </c>
-      <c r="J36" s="22" t="str">
+      <c r="J36" s="13" t="str">
         <v>Laptop</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="9">
         <f t="shared" ref="K36:K37" si="2">COUNTIF(B34:B53,J36)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="M36" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="25">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
       <c r="B37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="11">
         <v>750</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G37" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J37" s="22" t="str">
+      <c r="J37" s="13" t="str">
         <v>Phone</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="9">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="2:11">
+      <c r="M37" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="N37" s="25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
       <c r="B38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="11">
         <v>700</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="9">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="2:11">
+      <c r="M38" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="N38" s="25">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
       <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="11">
         <v>700</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:14">
       <c r="B40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="11">
         <v>640</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:14">
       <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="11">
         <v>620</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:14">
       <c r="B42" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="11">
         <v>600</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -1970,12 +4448,16 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="2:11">
+      <c r="I42" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="11">
         <v>550</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -1985,55 +4467,55 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:14">
       <c r="B44" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="11">
         <v>530</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:14">
       <c r="B45" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="11">
         <v>520</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:14">
       <c r="B46" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="11">
         <v>500</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:14">
       <c r="B47" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="11">
         <v>500</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
+    <row r="48" spans="2:14">
       <c r="B48" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="11">
         <v>480</v>
       </c>
       <c r="D48" s="7" t="s">
@@ -2044,7 +4526,7 @@
       <c r="B49" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="11">
         <v>450</v>
       </c>
       <c r="D49" s="7" t="s">
@@ -2055,7 +4537,7 @@
       <c r="B50" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="11">
         <v>410</v>
       </c>
       <c r="D50" s="7" t="s">
@@ -2066,7 +4548,7 @@
       <c r="B51" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="11">
         <v>400</v>
       </c>
       <c r="D51" s="7" t="s">
@@ -2077,7 +4559,7 @@
       <c r="B52" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="11">
         <v>300</v>
       </c>
       <c r="D52" s="7" t="s">
@@ -2089,7 +4571,14 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:D52">
     <sortCondition descending="1" ref="C33:C52"/>
   </sortState>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B4:H5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I10"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="F34:G34"/>
@@ -2098,15 +4587,9 @@
     <mergeCell ref="L8:M10"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G10"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B4:H5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I10"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C27">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2123,6 +4606,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId5"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
start a few project progress chart with todo list
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA22C1F0-9641-4A43-AA43-CBD6D255F81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B671ED8C-7F6E-4E48-9CB6-1CD9EADFD4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2712" yWindow="0" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="2" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
     <sheet name="PHASE1" sheetId="2" r:id="rId2"/>
     <sheet name="VIEW STUDENTS" sheetId="3" r:id="rId3"/>
+    <sheet name="PROGRESS" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PHASE1!$B$32:$D$52</definedName>
@@ -28,17 +29,17 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId7"/>
         <x14:slicerCache r:id="rId8"/>
         <x14:slicerCache r:id="rId9"/>
         <x14:slicerCache r:id="rId10"/>
+        <x14:slicerCache r:id="rId11"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="203">
   <si>
     <t>Day</t>
   </si>
@@ -1311,12 +1312,33 @@
   <si>
     <t>status</t>
   </si>
+  <si>
+    <t>TO DO LIST</t>
+  </si>
+  <si>
+    <t>STEP 1</t>
+  </si>
+  <si>
+    <t>STEP 2</t>
+  </si>
+  <si>
+    <t>STEP 3</t>
+  </si>
+  <si>
+    <t>STEP 4</t>
+  </si>
+  <si>
+    <t>STEP 5</t>
+  </si>
+  <si>
+    <t>STEP 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1458,6 +1480,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -1611,11 +1645,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1670,9 +1705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1724,62 +1756,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1795,6 +1795,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1823,44 +1829,80 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -2935,21 +2977,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'VIEW STUDENTS'!$R$39</c:f>
+              <c:f>'VIEW STUDENTS'!$R$39:$R$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Grand Total</c:v>
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'VIEW STUDENTS'!$S$39</c:f>
+              <c:f>'VIEW STUDENTS'!$S$39:$S$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3317,21 +3380,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'VIEW STUDENTS'!$T$39</c:f>
+              <c:f>'VIEW STUDENTS'!$T$39:$T$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Grand Total</c:v>
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'VIEW STUDENTS'!$U$39</c:f>
+              <c:f>'VIEW STUDENTS'!$U$39:$U$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3560,6 +3644,214 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26680387797131411"/>
+          <c:y val="0.14975915221579963"/>
+          <c:w val="0.44059530003039266"/>
+          <c:h val="0.65816417095261937"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>PROGRESS!$I$15:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D0E0-4A92-8752-BFD7476E78FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="75"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3717,6 +4009,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5716,6 +6048,549 @@
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6296,6 +7171,424 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>250371</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3153B70-10DB-499D-A906-479E3C478A65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>446049</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>178420</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3074" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3074"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52086989-7903-423A-8308-1DE0FBEB5216}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3075" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3075"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A75F294-67BE-498D-A644-B89B1BE72414}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3076" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3076"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BCBF4C5-62A1-4B19-94B7-22DE0C4FCC1C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3077" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3077"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5038C94-8BE6-4168-80F0-422D6C3657DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>226740</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>3718</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3078" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3078"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45F8994-423C-47ED-BF58-3A9AECBDBD5E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -7063,7 +8356,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6508D488-2093-44C4-8172-E3F115C3FCE6}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="T38:U39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="T38:U43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
       <items count="21">
@@ -7094,9 +8387,9 @@
     <pivotField showAll="0">
       <items count="5">
         <item h="1" x="0"/>
-        <item x="3"/>
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7105,8 +8398,8 @@
     <pivotField showAll="0">
       <items count="4">
         <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7115,7 +8408,7 @@
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7123,7 +8416,19 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="1">
+  <rowItems count="5">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -7159,7 +8464,7 @@
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A1EADDD7-A2EB-43B0-909C-0F2366B57B7F}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="R38:S39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="R38:S43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
       <items count="21">
@@ -7214,9 +8519,9 @@
     <pivotField showAll="0">
       <items count="5">
         <item h="1" x="0"/>
-        <item x="3"/>
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7225,8 +8530,8 @@
     <pivotField showAll="0">
       <items count="4">
         <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7235,7 +8540,7 @@
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7243,7 +8548,19 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="1">
+  <rowItems count="5">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -7305,8 +8622,8 @@
     <tabular pivotCacheId="265272106">
       <items count="3">
         <i x="2"/>
-        <i x="1"/>
-        <i x="0" s="1" nd="1"/>
+        <i x="1" s="1"/>
+        <i x="0"/>
       </items>
     </tabular>
   </data>
@@ -7323,9 +8640,9 @@
     <tabular pivotCacheId="265272106">
       <items count="4">
         <i x="0"/>
-        <i x="2"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="1" nd="1"/>
+        <i x="3"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -7341,8 +8658,8 @@
   <data>
     <tabular pivotCacheId="265272106">
       <items count="2">
-        <i x="1"/>
-        <i x="0" s="1" nd="1"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
       </items>
     </tabular>
   </data>
@@ -7708,13 +9025,13 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="60.6" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -7832,44 +9149,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -7881,22 +9198,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="65" t="s">
+      <c r="G7" s="72"/>
+      <c r="H7" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65" t="s">
+      <c r="I7" s="61"/>
+      <c r="J7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65" t="s">
+      <c r="K7" s="61"/>
+      <c r="L7" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="65"/>
+      <c r="M7" s="61"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -7909,26 +9226,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="64">
+      <c r="F8" s="62">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64">
+      <c r="I8" s="62"/>
+      <c r="J8" s="62">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64">
+      <c r="K8" s="62"/>
+      <c r="L8" s="62">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="64"/>
+      <c r="M8" s="62"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -7941,14 +9258,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -7961,14 +9278,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -8023,10 +9340,10 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="F14" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="74"/>
+      <c r="G14" s="65"/>
       <c r="K14" s="15" t="s">
         <v>66</v>
       </c>
@@ -8209,15 +9526,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="10" t="s">
@@ -8251,14 +9568,14 @@
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="77" t="s">
+      <c r="F34" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="77"/>
-      <c r="J34" s="77" t="s">
+      <c r="G34" s="68"/>
+      <c r="J34" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="77"/>
+      <c r="K34" s="68"/>
       <c r="M34" s="14" t="s">
         <v>86</v>
       </c>
@@ -8430,10 +9747,10 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="73" t="s">
+      <c r="I42" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="73"/>
+      <c r="J42" s="64"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
@@ -8549,11 +9866,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.6">
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
       <c r="E57" s="17"/>
       <c r="H57">
         <v>123</v>
@@ -8563,9 +9880,9 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
       <c r="E58" s="17"/>
       <c r="H58">
         <v>124</v>
@@ -8583,11 +9900,11 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="78" t="s">
+      <c r="B60" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="78"/>
-      <c r="D60" s="78"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="69"/>
       <c r="H60">
         <v>126</v>
       </c>
@@ -8599,10 +9916,10 @@
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="79" t="s">
+      <c r="C61" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="80"/>
+      <c r="D61" s="71"/>
       <c r="H61">
         <v>127</v>
       </c>
@@ -8614,10 +9931,10 @@
       <c r="B62" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="61" t="s">
+      <c r="C62" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="62"/>
+      <c r="D62" s="74"/>
       <c r="H62">
         <v>128</v>
       </c>
@@ -8629,10 +9946,10 @@
       <c r="B63" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="61" t="s">
+      <c r="C63" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="62"/>
+      <c r="D63" s="74"/>
       <c r="H63">
         <v>129</v>
       </c>
@@ -8644,10 +9961,10 @@
       <c r="B64" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="61" t="s">
+      <c r="C64" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="62"/>
+      <c r="D64" s="74"/>
       <c r="H64">
         <v>130</v>
       </c>
@@ -8672,10 +9989,10 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="B67" s="63" t="s">
+      <c r="B67" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="63"/>
+      <c r="C67" s="75"/>
       <c r="D67" s="9">
         <v>34</v>
       </c>
@@ -8687,10 +10004,10 @@
       </c>
     </row>
     <row r="68" spans="2:10">
-      <c r="B68" s="63" t="s">
+      <c r="B68" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="63"/>
+      <c r="C68" s="75"/>
       <c r="D68" s="9">
         <v>35</v>
       </c>
@@ -8702,10 +10019,10 @@
       </c>
     </row>
     <row r="69" spans="2:10">
-      <c r="B69" s="63" t="s">
+      <c r="B69" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="63"/>
+      <c r="C69" s="75"/>
       <c r="D69" s="9">
         <v>36</v>
       </c>
@@ -8720,10 +10037,10 @@
       </c>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="63" t="s">
+      <c r="B70" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="C70" s="63"/>
+      <c r="C70" s="75"/>
       <c r="D70" s="9">
         <v>37</v>
       </c>
@@ -8735,10 +10052,10 @@
       </c>
     </row>
     <row r="71" spans="2:10">
-      <c r="B71" s="63" t="s">
+      <c r="B71" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="C71" s="63"/>
+      <c r="C71" s="75"/>
       <c r="D71" s="9">
         <v>38</v>
       </c>
@@ -8750,10 +10067,10 @@
       </c>
     </row>
     <row r="72" spans="2:10">
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="63"/>
+      <c r="C72" s="75"/>
       <c r="D72" s="9">
         <v>39</v>
       </c>
@@ -8765,10 +10082,10 @@
       </c>
     </row>
     <row r="73" spans="2:10">
-      <c r="B73" s="63" t="s">
+      <c r="B73" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="63"/>
+      <c r="C73" s="75"/>
       <c r="D73" s="9">
         <v>40</v>
       </c>
@@ -8820,18 +10137,18 @@
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="67" t="s">
+      <c r="B81" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="67"/>
-      <c r="D81" s="67"/>
-      <c r="E81" s="67"/>
+      <c r="C81" s="56"/>
+      <c r="D81" s="56"/>
+      <c r="E81" s="56"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="67"/>
-      <c r="C82" s="67"/>
-      <c r="D82" s="67"/>
-      <c r="E82" s="67"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="56"/>
+      <c r="E82" s="56"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="10" t="s">
@@ -8922,18 +10239,18 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="68" t="s">
+      <c r="B97" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="68"/>
-      <c r="D97" s="68"/>
-      <c r="E97" s="68"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="57"/>
+      <c r="E97" s="57"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="68"/>
-      <c r="C98" s="68"/>
-      <c r="D98" s="68"/>
-      <c r="E98" s="68"/>
+      <c r="B98" s="57"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="10" t="s">
@@ -9024,22 +10341,22 @@
       </c>
     </row>
     <row r="114" spans="2:14">
-      <c r="B114" s="69" t="s">
+      <c r="B114" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="69"/>
-      <c r="D114" s="69"/>
-      <c r="E114" s="69"/>
-      <c r="F114" s="69"/>
-      <c r="G114" s="69"/>
+      <c r="C114" s="58"/>
+      <c r="D114" s="58"/>
+      <c r="E114" s="58"/>
+      <c r="F114" s="58"/>
+      <c r="G114" s="58"/>
     </row>
     <row r="115" spans="2:14">
-      <c r="B115" s="69"/>
-      <c r="C115" s="69"/>
-      <c r="D115" s="69"/>
-      <c r="E115" s="69"/>
-      <c r="F115" s="69"/>
-      <c r="G115" s="69"/>
+      <c r="B115" s="58"/>
+      <c r="C115" s="58"/>
+      <c r="D115" s="58"/>
+      <c r="E115" s="58"/>
+      <c r="F115" s="58"/>
+      <c r="G115" s="58"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="10" t="s">
@@ -9057,13 +10374,13 @@
       <c r="H117" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="J117" s="28" t="s">
+      <c r="J117" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="K117" s="28" t="s">
+      <c r="K117" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="L117" s="28" t="s">
+      <c r="L117" s="27" t="s">
         <v>121</v>
       </c>
     </row>
@@ -9089,7 +10406,7 @@
         <f>SUMIF(D118:D127,F118,C118:C127)</f>
         <v>1750</v>
       </c>
-      <c r="J118" s="29" t="s">
+      <c r="J118" s="28" t="s">
         <v>119</v>
       </c>
       <c r="K118" s="9">
@@ -9144,11 +10461,11 @@
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="L120" s="55" t="s">
+      <c r="L120" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="M120" s="56"/>
-      <c r="N120" s="56"/>
+      <c r="M120" s="78"/>
+      <c r="N120" s="78"/>
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="3" t="s">
@@ -9171,9 +10488,9 @@
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="L121" s="56"/>
-      <c r="M121" s="56"/>
-      <c r="N121" s="56"/>
+      <c r="L121" s="78"/>
+      <c r="M121" s="78"/>
+      <c r="N121" s="78"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="3" t="s">
@@ -9196,10 +10513,10 @@
       <c r="D123" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J123" s="54" t="s">
+      <c r="J123" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="K123" s="54"/>
+      <c r="K123" s="76"/>
       <c r="L123" s="21" t="str" cm="1">
         <f t="array" ref="L123:L125">_xlfn.UNIQUE(B118:B127)</f>
         <v>Laptop</v>
@@ -9256,20 +10573,20 @@
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="68" t="s">
+      <c r="B130" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="68"/>
-      <c r="D130" s="68"/>
-      <c r="E130" s="68"/>
-      <c r="F130" s="68"/>
+      <c r="C130" s="57"/>
+      <c r="D130" s="57"/>
+      <c r="E130" s="57"/>
+      <c r="F130" s="57"/>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" s="68"/>
-      <c r="C131" s="68"/>
-      <c r="D131" s="68"/>
-      <c r="E131" s="68"/>
-      <c r="F131" s="68"/>
+      <c r="B131" s="57"/>
+      <c r="C131" s="57"/>
+      <c r="D131" s="57"/>
+      <c r="E131" s="57"/>
+      <c r="F131" s="57"/>
     </row>
     <row r="133" spans="2:11">
       <c r="B133" s="10" t="s">
@@ -9284,7 +10601,7 @@
       <c r="E133" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="I133" s="27" t="s">
+      <c r="I133" s="26" t="s">
         <v>124</v>
       </c>
     </row>
@@ -9311,13 +10628,13 @@
         <v>74</v>
       </c>
       <c r="E135" s="3"/>
-      <c r="I135" s="30" t="s">
+      <c r="I135" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="J135" s="57" t="s">
+      <c r="J135" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="58"/>
+      <c r="K135" s="80"/>
     </row>
     <row r="136" spans="2:11">
       <c r="B136" s="3" t="s">
@@ -9330,14 +10647,14 @@
         <v>72</v>
       </c>
       <c r="E136" s="3"/>
-      <c r="I136" s="30" t="s">
+      <c r="I136" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J136" s="57">
+      <c r="J136" s="79">
         <f>IFERROR(VLOOKUP($J$135,$B$134:$D$143,2,FALSE),"Not found")</f>
         <v>300</v>
       </c>
-      <c r="K136" s="58"/>
+      <c r="K136" s="80"/>
     </row>
     <row r="137" spans="2:11">
       <c r="B137" s="3" t="s">
@@ -9436,10 +10753,10 @@
       <c r="E146" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="59" t="s">
+      <c r="G146" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="H146" s="60"/>
+      <c r="H146" s="82"/>
     </row>
     <row r="147" spans="2:10" ht="16.8" customHeight="1">
       <c r="B147" s="3" t="s">
@@ -9454,14 +10771,14 @@
       <c r="E147" s="3">
         <v>85</v>
       </c>
-      <c r="G147" s="51" t="s">
+      <c r="G147" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="H147" s="51"/>
-      <c r="I147" s="52" t="s">
+      <c r="H147" s="84"/>
+      <c r="I147" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="J147" s="52"/>
+      <c r="J147" s="85"/>
     </row>
     <row r="148" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B148" s="3" t="s">
@@ -9476,11 +10793,11 @@
       <c r="E148" s="3">
         <v>78</v>
       </c>
-      <c r="I148" s="53" t="str">
+      <c r="I148" s="86" t="str">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,2,FALSE),"NOT FOUND")</f>
         <v>charlie@email.com</v>
       </c>
-      <c r="J148" s="53"/>
+      <c r="J148" s="86"/>
     </row>
     <row r="149" spans="2:10" ht="22.2" customHeight="1">
       <c r="B149" s="3" t="s">
@@ -9495,11 +10812,11 @@
       <c r="E149" s="3">
         <v>92</v>
       </c>
-      <c r="I149" s="53">
+      <c r="I149" s="86">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,3,FALSE),"NOT FOUND")</f>
         <v>7654321098</v>
       </c>
-      <c r="J149" s="53"/>
+      <c r="J149" s="86"/>
     </row>
     <row r="150" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B150" s="3" t="s">
@@ -9514,11 +10831,11 @@
       <c r="E150" s="3">
         <v>67</v>
       </c>
-      <c r="I150" s="53">
+      <c r="I150" s="86">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,4,FALSE),"NOT FOUND")</f>
         <v>92</v>
       </c>
-      <c r="J150" s="53"/>
+      <c r="J150" s="86"/>
     </row>
     <row r="151" spans="2:10" ht="21.6" customHeight="1">
       <c r="B151" s="3" t="s">
@@ -9533,8 +10850,8 @@
       <c r="E151" s="3">
         <v>74</v>
       </c>
-      <c r="I151" s="50"/>
-      <c r="J151" s="50"/>
+      <c r="I151" s="83"/>
+      <c r="J151" s="83"/>
     </row>
     <row r="152" spans="2:10" ht="21.6" customHeight="1"/>
   </sheetData>
@@ -9543,6 +10860,33 @@
     <sortCondition descending="1" ref="C33:C52"/>
   </sortState>
   <mergeCells count="43">
+    <mergeCell ref="I151:J151"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="I147:J147"/>
+    <mergeCell ref="I148:J148"/>
+    <mergeCell ref="I149:J149"/>
+    <mergeCell ref="I150:J150"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="L120:N121"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G10"/>
     <mergeCell ref="B81:E82"/>
     <mergeCell ref="B97:E98"/>
     <mergeCell ref="B114:G115"/>
@@ -9559,33 +10903,6 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="C61:D61"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G10"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="L120:N121"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="I151:J151"/>
-    <mergeCell ref="G147:H147"/>
-    <mergeCell ref="I147:J147"/>
-    <mergeCell ref="I148:J148"/>
-    <mergeCell ref="I149:J149"/>
-    <mergeCell ref="I150:J150"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="C8:C27">
@@ -9809,8 +11126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35914A46-0205-471D-B2D7-66681A3205BE}">
   <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P82" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView topLeftCell="P44" workbookViewId="0">
+      <selection activeCell="AH74" sqref="AH74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9829,19 +11146,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>140</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
     </row>
     <row r="5" spans="1:5" ht="15.6">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>141</v>
       </c>
       <c r="B5" s="21"/>
@@ -9850,130 +11167,130 @@
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="32"/>
+      <c r="A6" s="31"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="35"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="35"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="35"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="35"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="35"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="35"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="35"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="35"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
     </row>
     <row r="25" spans="1:5" ht="15.6">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>142</v>
       </c>
       <c r="B25" s="21"/>
@@ -9981,80 +11298,80 @@
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="32"/>
+      <c r="A26" s="31"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="35"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="35"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="35"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="35"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="20" t="s">
@@ -10087,11 +11404,11 @@
       <c r="J38" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="82" t="s">
+      <c r="L38" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="M38" s="82"/>
-      <c r="N38" s="82"/>
+      <c r="M38" s="91"/>
+      <c r="N38" s="91"/>
       <c r="R38" s="14" t="s">
         <v>86</v>
       </c>
@@ -10106,435 +11423,487 @@
       </c>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="38">
+      <c r="A39" s="37">
         <v>104</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="37">
         <v>22</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="37">
         <v>6543210987</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="37">
         <v>11</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="37">
         <v>67</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="37">
         <v>85</v>
       </c>
-      <c r="I39" s="38" t="s">
+      <c r="I39" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J39" t="str">
         <f>IF(AND(G39&gt;70,I39="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="N39" s="82"/>
-      <c r="R39" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="S39" s="16"/>
-      <c r="T39" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="U39" s="16"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="91"/>
+      <c r="N39" s="91"/>
+      <c r="R39" s="47">
+        <v>104</v>
+      </c>
+      <c r="S39" s="16">
+        <v>67</v>
+      </c>
+      <c r="T39" s="47">
+        <v>104</v>
+      </c>
+      <c r="U39" s="16">
+        <v>85</v>
+      </c>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="38">
+      <c r="A40" s="37">
         <v>112</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="38">
+      <c r="C40" s="37">
         <v>22</v>
       </c>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="E40" s="38">
+      <c r="E40" s="37">
         <v>7654302109</v>
       </c>
-      <c r="F40" s="38">
+      <c r="F40" s="37">
         <v>11</v>
       </c>
-      <c r="G40" s="38">
+      <c r="G40" s="37">
         <v>73</v>
       </c>
-      <c r="H40" s="38">
+      <c r="H40" s="37">
         <v>91</v>
       </c>
-      <c r="I40" s="38" t="s">
+      <c r="I40" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" ref="J40:J58" si="0">IF(AND(G40&gt;70,I40="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L40" s="81" t="s">
+      <c r="L40" s="92" t="s">
         <v>194</v>
       </c>
-      <c r="M40" s="81"/>
-      <c r="N40" s="81"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="92"/>
+      <c r="R40" s="47">
+        <v>108</v>
+      </c>
+      <c r="S40" s="16">
+        <v>95</v>
+      </c>
+      <c r="T40" s="47">
+        <v>108</v>
+      </c>
+      <c r="U40" s="16">
+        <v>92</v>
+      </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="38">
+      <c r="A41" s="37">
         <v>105</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="38">
+      <c r="C41" s="37">
         <v>20</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E41" s="38">
+      <c r="E41" s="37">
         <v>5432109876</v>
       </c>
-      <c r="F41" s="38">
+      <c r="F41" s="37">
         <v>11</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="37">
         <v>74</v>
       </c>
-      <c r="H41" s="38">
+      <c r="H41" s="37">
         <v>87</v>
       </c>
-      <c r="I41" s="38" t="s">
+      <c r="I41" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="M41" s="81">
+      <c r="M41" s="92">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,2,FALSE),"Not found")</f>
         <v>22</v>
       </c>
-      <c r="N41" s="81"/>
+      <c r="N41" s="92"/>
+      <c r="R41" s="47">
+        <v>112</v>
+      </c>
+      <c r="S41" s="16">
+        <v>73</v>
+      </c>
+      <c r="T41" s="47">
+        <v>112</v>
+      </c>
+      <c r="U41" s="16">
+        <v>91</v>
+      </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="38">
+      <c r="A42" s="37">
         <v>117</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="38">
+      <c r="C42" s="37">
         <v>20</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="E42" s="38">
+      <c r="E42" s="37">
         <v>2109876541</v>
       </c>
-      <c r="F42" s="38">
+      <c r="F42" s="37">
         <v>11</v>
       </c>
-      <c r="G42" s="38">
+      <c r="G42" s="37">
         <v>76</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H42" s="37">
         <v>88</v>
       </c>
-      <c r="I42" s="38" t="s">
+      <c r="I42" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
         <v>pending</v>
       </c>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="81" t="str">
+      <c r="M42" s="92" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,3,FALSE),"Not found")</f>
         <v>david@email.com</v>
       </c>
-      <c r="N42" s="81"/>
+      <c r="N42" s="92"/>
+      <c r="R42" s="47">
+        <v>120</v>
+      </c>
+      <c r="S42" s="16">
+        <v>85</v>
+      </c>
+      <c r="T42" s="47">
+        <v>120</v>
+      </c>
+      <c r="U42" s="16">
+        <v>84</v>
+      </c>
     </row>
     <row r="43" spans="1:21">
-      <c r="A43" s="38">
+      <c r="A43" s="37">
         <v>110</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="38">
+      <c r="C43" s="37">
         <v>21</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="E43" s="38">
+      <c r="E43" s="37">
         <v>9876504321</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F43" s="37">
         <v>12</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="37">
         <v>77</v>
       </c>
-      <c r="H43" s="38">
+      <c r="H43" s="37">
         <v>85</v>
       </c>
-      <c r="I43" s="38" t="s">
+      <c r="I43" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
         <v>pending</v>
       </c>
-      <c r="L43" s="29" t="s">
+      <c r="L43" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="81">
+      <c r="M43" s="92">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,4,FALSE),"Not found")</f>
         <v>6543210987</v>
       </c>
-      <c r="N43" s="81"/>
+      <c r="N43" s="92"/>
+      <c r="R43" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="S43" s="16">
+        <v>320</v>
+      </c>
+      <c r="T43" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="U43" s="16">
+        <v>352</v>
+      </c>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="38">
+      <c r="A44" s="37">
         <v>102</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="38">
+      <c r="C44" s="37">
         <v>21</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="38">
+      <c r="E44" s="37">
         <v>8765432109</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="37">
         <v>10</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="37">
         <v>78</v>
       </c>
-      <c r="H44" s="38">
+      <c r="H44" s="37">
         <v>90</v>
       </c>
-      <c r="I44" s="38" t="s">
+      <c r="I44" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L44" s="29" t="s">
+      <c r="L44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M44" s="81">
+      <c r="M44" s="92">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,5,FALSE),"Not found")</f>
         <v>11</v>
       </c>
-      <c r="N44" s="81"/>
+      <c r="N44" s="92"/>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="38">
+      <c r="A45" s="37">
         <v>113</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="38">
+      <c r="C45" s="37">
         <v>20</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="E45" s="38">
+      <c r="E45" s="37">
         <v>6543201098</v>
       </c>
-      <c r="F45" s="38">
+      <c r="F45" s="37">
         <v>12</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="37">
         <v>79</v>
       </c>
-      <c r="H45" s="38">
+      <c r="H45" s="37">
         <v>89</v>
       </c>
-      <c r="I45" s="38" t="s">
+      <c r="I45" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L45" s="29" t="s">
+      <c r="L45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="81">
+      <c r="M45" s="92">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,6,FALSE),"Not found")</f>
         <v>67</v>
       </c>
-      <c r="N45" s="81"/>
+      <c r="N45" s="92"/>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46" s="38">
+      <c r="A46" s="37">
         <v>116</v>
       </c>
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="38">
+      <c r="C46" s="37">
         <v>22</v>
       </c>
-      <c r="D46" s="39" t="s">
+      <c r="D46" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="E46" s="38">
+      <c r="E46" s="37">
         <v>3210987652</v>
       </c>
-      <c r="F46" s="38">
+      <c r="F46" s="37">
         <v>12</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="37">
         <v>81</v>
       </c>
-      <c r="H46" s="38">
+      <c r="H46" s="37">
         <v>82</v>
       </c>
-      <c r="I46" s="38" t="s">
+      <c r="I46" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L46" s="37" t="s">
+      <c r="L46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="M46" s="81">
+      <c r="M46" s="92">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,7,FALSE),"Not found")</f>
         <v>85</v>
       </c>
-      <c r="N46" s="81"/>
+      <c r="N46" s="92"/>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="38">
+      <c r="A47" s="37">
         <v>111</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="C47" s="38">
+      <c r="C47" s="37">
         <v>19</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="E47" s="38">
+      <c r="E47" s="37">
         <v>8765403210</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F47" s="37">
         <v>10</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="37">
         <v>82</v>
       </c>
-      <c r="H47" s="38">
+      <c r="H47" s="37">
         <v>96</v>
       </c>
-      <c r="I47" s="38" t="s">
+      <c r="I47" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L47" s="29" t="s">
+      <c r="L47" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="81" t="str">
+      <c r="M47" s="92" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,8,FALSE),"Not found")</f>
         <v>No</v>
       </c>
-      <c r="N47" s="81"/>
+      <c r="N47" s="92"/>
     </row>
     <row r="48" spans="1:21">
-      <c r="A48" s="38">
+      <c r="A48" s="37">
         <v>118</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="38">
+      <c r="C48" s="37">
         <v>21</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D48" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="38">
+      <c r="E48" s="37">
         <v>1098765430</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="37">
         <v>10</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="37">
         <v>83</v>
       </c>
-      <c r="H48" s="38">
+      <c r="H48" s="37">
         <v>95</v>
       </c>
-      <c r="I48" s="38" t="s">
+      <c r="I48" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="M48" s="50"/>
-      <c r="N48" s="50"/>
+      <c r="M48" s="83"/>
+      <c r="N48" s="83"/>
     </row>
     <row r="49" spans="1:15">
-      <c r="A49" s="38">
+      <c r="A49" s="37">
         <v>120</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="38">
+      <c r="C49" s="37">
         <v>22</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D49" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="E49" s="38">
+      <c r="E49" s="37">
         <v>8765432102</v>
       </c>
-      <c r="F49" s="38">
+      <c r="F49" s="37">
         <v>11</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="37">
         <v>85</v>
       </c>
-      <c r="H49" s="38">
+      <c r="H49" s="37">
         <v>84</v>
       </c>
-      <c r="I49" s="38" t="s">
+      <c r="I49" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J49" t="str">
@@ -10543,38 +11912,38 @@
       </c>
     </row>
     <row r="50" spans="1:15">
-      <c r="A50" s="38">
+      <c r="A50" s="37">
         <v>101</v>
       </c>
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="38">
+      <c r="C50" s="37">
         <v>20</v>
       </c>
-      <c r="D50" s="39" t="s">
+      <c r="D50" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E50" s="38">
+      <c r="E50" s="37">
         <v>9876543210</v>
       </c>
-      <c r="F50" s="38">
+      <c r="F50" s="37">
         <v>10</v>
       </c>
-      <c r="G50" s="38">
+      <c r="G50" s="37">
         <v>85</v>
       </c>
-      <c r="H50" s="38">
+      <c r="H50" s="37">
         <v>95</v>
       </c>
-      <c r="I50" s="38" t="s">
+      <c r="I50" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
         <v>pending</v>
       </c>
-      <c r="L50" s="43" t="s">
+      <c r="L50" s="42" t="s">
         <v>188</v>
       </c>
       <c r="M50" s="21" t="s">
@@ -10588,31 +11957,31 @@
       </c>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="38">
+      <c r="A51" s="37">
         <v>114</v>
       </c>
-      <c r="B51" s="39" t="s">
+      <c r="B51" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C51" s="38">
+      <c r="C51" s="37">
         <v>21</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="D51" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="E51" s="38">
+      <c r="E51" s="37">
         <v>5432109870</v>
       </c>
-      <c r="F51" s="38">
+      <c r="F51" s="37">
         <v>10</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="37">
         <v>86</v>
       </c>
-      <c r="H51" s="38">
+      <c r="H51" s="37">
         <v>93</v>
       </c>
-      <c r="I51" s="38" t="s">
+      <c r="I51" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J51" t="str">
@@ -10627,7 +11996,7 @@
         <f t="array" ref="M51:M53">_xlfn.UNIQUE(F39:F58)</f>
         <v>11</v>
       </c>
-      <c r="N51" s="45" cm="1">
+      <c r="N51" s="44" cm="1">
         <f t="array" ref="N51:N69">_xlfn.UNIQUE(G39:G58)</f>
         <v>67</v>
       </c>
@@ -10637,31 +12006,31 @@
       </c>
     </row>
     <row r="52" spans="1:15">
-      <c r="A52" s="38">
+      <c r="A52" s="37">
         <v>119</v>
       </c>
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="38">
+      <c r="C52" s="37">
         <v>19</v>
       </c>
-      <c r="D52" s="39" t="s">
+      <c r="D52" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="E52" s="38">
+      <c r="E52" s="37">
         <v>9876543201</v>
       </c>
-      <c r="F52" s="38">
+      <c r="F52" s="37">
         <v>12</v>
       </c>
-      <c r="G52" s="38">
+      <c r="G52" s="37">
         <v>87</v>
       </c>
-      <c r="H52" s="38">
+      <c r="H52" s="37">
         <v>90</v>
       </c>
-      <c r="I52" s="38" t="s">
+      <c r="I52" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J52" t="str">
@@ -10674,7 +12043,7 @@
       <c r="M52">
         <v>12</v>
       </c>
-      <c r="N52" s="45">
+      <c r="N52" s="44">
         <v>73</v>
       </c>
       <c r="O52">
@@ -10682,44 +12051,44 @@
       </c>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="38">
+      <c r="A53" s="37">
         <v>106</v>
       </c>
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="38">
+      <c r="C53" s="37">
         <v>21</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E53" s="37">
         <v>4321098765</v>
       </c>
-      <c r="F53" s="38">
+      <c r="F53" s="37">
         <v>12</v>
       </c>
-      <c r="G53" s="38">
+      <c r="G53" s="37">
         <v>88</v>
       </c>
-      <c r="H53" s="38">
+      <c r="H53" s="37">
         <v>90</v>
       </c>
-      <c r="I53" s="38" t="s">
+      <c r="I53" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L53" s="44">
+      <c r="L53" s="43">
         <v>21</v>
       </c>
-      <c r="M53" s="40">
+      <c r="M53" s="39">
         <v>10</v>
       </c>
-      <c r="N53" s="46">
+      <c r="N53" s="45">
         <v>74</v>
       </c>
       <c r="O53">
@@ -10727,42 +12096,42 @@
       </c>
     </row>
     <row r="54" spans="1:15">
-      <c r="A54" s="38">
+      <c r="A54" s="37">
         <v>109</v>
       </c>
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="C54" s="38">
+      <c r="C54" s="37">
         <v>20</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E54" s="38">
+      <c r="E54" s="37">
         <v>1098765432</v>
       </c>
-      <c r="F54" s="38">
+      <c r="F54" s="37">
         <v>10</v>
       </c>
-      <c r="G54" s="38">
+      <c r="G54" s="37">
         <v>89</v>
       </c>
-      <c r="H54" s="38">
+      <c r="H54" s="37">
         <v>97</v>
       </c>
-      <c r="I54" s="38" t="s">
+      <c r="I54" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L54" s="42">
+      <c r="L54" s="41">
         <v>19</v>
       </c>
-      <c r="M54" s="42"/>
-      <c r="N54" s="47">
+      <c r="M54" s="41"/>
+      <c r="N54" s="46">
         <v>76</v>
       </c>
       <c r="O54">
@@ -10770,40 +12139,40 @@
       </c>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="38">
+      <c r="A55" s="37">
         <v>115</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C55" s="38">
+      <c r="C55" s="37">
         <v>19</v>
       </c>
-      <c r="D55" s="39" t="s">
+      <c r="D55" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="E55" s="38">
+      <c r="E55" s="37">
         <v>4321098761</v>
       </c>
-      <c r="F55" s="38">
+      <c r="F55" s="37">
         <v>11</v>
       </c>
-      <c r="G55" s="38">
+      <c r="G55" s="37">
         <v>90</v>
       </c>
-      <c r="H55" s="38">
+      <c r="H55" s="37">
         <v>94</v>
       </c>
-      <c r="I55" s="38" t="s">
+      <c r="I55" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
         <v>pending</v>
       </c>
-      <c r="L55" s="41"/>
-      <c r="M55" s="42"/>
-      <c r="N55" s="47">
+      <c r="L55" s="40"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="46">
         <v>77</v>
       </c>
       <c r="O55">
@@ -10811,40 +12180,40 @@
       </c>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="38">
+      <c r="A56" s="37">
         <v>107</v>
       </c>
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="37">
         <v>19</v>
       </c>
-      <c r="D56" s="39" t="s">
+      <c r="D56" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="E56" s="38">
+      <c r="E56" s="37">
         <v>3210987654</v>
       </c>
-      <c r="F56" s="38">
+      <c r="F56" s="37">
         <v>12</v>
       </c>
-      <c r="G56" s="38">
+      <c r="G56" s="37">
         <v>91</v>
       </c>
-      <c r="H56" s="38">
+      <c r="H56" s="37">
         <v>80</v>
       </c>
-      <c r="I56" s="38" t="s">
+      <c r="I56" s="37" t="s">
         <v>161</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
         <v>pending</v>
       </c>
-      <c r="L56" s="41"/>
-      <c r="M56" s="42"/>
-      <c r="N56" s="47">
+      <c r="L56" s="40"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="46">
         <v>78</v>
       </c>
       <c r="O56">
@@ -10852,40 +12221,40 @@
       </c>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="38">
+      <c r="A57" s="37">
         <v>103</v>
       </c>
-      <c r="B57" s="39" t="s">
+      <c r="B57" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C57" s="38">
+      <c r="C57" s="37">
         <v>19</v>
       </c>
-      <c r="D57" s="39" t="s">
+      <c r="D57" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="38">
+      <c r="E57" s="37">
         <v>7654321098</v>
       </c>
-      <c r="F57" s="38">
+      <c r="F57" s="37">
         <v>10</v>
       </c>
-      <c r="G57" s="38">
+      <c r="G57" s="37">
         <v>92</v>
       </c>
-      <c r="H57" s="38">
+      <c r="H57" s="37">
         <v>88</v>
       </c>
-      <c r="I57" s="38" t="s">
+      <c r="I57" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="L57" s="41"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="47">
+      <c r="L57" s="40"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="46">
         <v>79</v>
       </c>
       <c r="O57">
@@ -10893,38 +12262,38 @@
       </c>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="38">
+      <c r="A58" s="37">
         <v>108</v>
       </c>
-      <c r="B58" s="39" t="s">
+      <c r="B58" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="C58" s="38">
+      <c r="C58" s="37">
         <v>22</v>
       </c>
-      <c r="D58" s="39" t="s">
+      <c r="D58" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="38">
+      <c r="E58" s="37">
         <v>2109876543</v>
       </c>
-      <c r="F58" s="38">
+      <c r="F58" s="37">
         <v>11</v>
       </c>
-      <c r="G58" s="38">
+      <c r="G58" s="37">
         <v>95</v>
       </c>
-      <c r="H58" s="38">
+      <c r="H58" s="37">
         <v>92</v>
       </c>
-      <c r="I58" s="38" t="s">
+      <c r="I58" s="37" t="s">
         <v>160</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="N58" s="45">
+      <c r="N58" s="44">
         <v>81</v>
       </c>
       <c r="O58">
@@ -10932,7 +12301,7 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="N59" s="45">
+      <c r="N59" s="44">
         <v>82</v>
       </c>
       <c r="O59">
@@ -10940,7 +12309,7 @@
       </c>
     </row>
     <row r="60" spans="1:15">
-      <c r="N60" s="45">
+      <c r="N60" s="44">
         <v>83</v>
       </c>
       <c r="O60">
@@ -10948,7 +12317,7 @@
       </c>
     </row>
     <row r="61" spans="1:15">
-      <c r="N61" s="45">
+      <c r="N61" s="44">
         <v>85</v>
       </c>
       <c r="O61">
@@ -10956,7 +12325,7 @@
       </c>
     </row>
     <row r="62" spans="1:15">
-      <c r="N62" s="45">
+      <c r="N62" s="44">
         <v>86</v>
       </c>
       <c r="O62">
@@ -10964,7 +12333,7 @@
       </c>
     </row>
     <row r="63" spans="1:15">
-      <c r="N63" s="45">
+      <c r="N63" s="44">
         <v>87</v>
       </c>
       <c r="O63">
@@ -10972,7 +12341,7 @@
       </c>
     </row>
     <row r="64" spans="1:15">
-      <c r="N64" s="45">
+      <c r="N64" s="44">
         <v>88</v>
       </c>
       <c r="O64">
@@ -10980,7 +12349,7 @@
       </c>
     </row>
     <row r="65" spans="1:15">
-      <c r="N65" s="45">
+      <c r="N65" s="44">
         <v>89</v>
       </c>
       <c r="O65">
@@ -10988,115 +12357,115 @@
       </c>
     </row>
     <row r="66" spans="1:15">
-      <c r="N66" s="45">
+      <c r="N66" s="44">
         <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:15">
-      <c r="N67" s="45">
+      <c r="N67" s="44">
         <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="15" customHeight="1">
-      <c r="A68" s="84" t="s">
+      <c r="A68" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="B68" s="86" t="s">
+      <c r="B68" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="88" t="s">
+      <c r="C68" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="D68" s="90" t="s">
+      <c r="D68" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="85">
+      <c r="F68" s="88">
         <v>103</v>
       </c>
-      <c r="G68" s="85"/>
-      <c r="N68" s="45">
+      <c r="G68" s="88"/>
+      <c r="N68" s="44">
         <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:15">
-      <c r="A69" s="83">
+      <c r="A69" s="48">
         <v>101</v>
       </c>
-      <c r="B69" s="83" t="s">
+      <c r="B69" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="83">
+      <c r="C69" s="48">
         <v>20</v>
       </c>
-      <c r="D69" s="83">
+      <c r="D69" s="48">
         <v>85</v>
       </c>
-      <c r="F69" s="87" t="str">
+      <c r="F69" s="89" t="str">
         <f>VLOOKUP($F$68,$A$68:$D$71,2,FALSE)</f>
         <v>Charlie</v>
       </c>
-      <c r="G69" s="87"/>
-      <c r="N69" s="45">
+      <c r="G69" s="89"/>
+      <c r="N69" s="44">
         <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:15">
-      <c r="A70" s="83">
+      <c r="A70" s="48">
         <v>102</v>
       </c>
-      <c r="B70" s="83" t="s">
+      <c r="B70" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="83">
+      <c r="C70" s="48">
         <v>21</v>
       </c>
-      <c r="D70" s="83">
+      <c r="D70" s="48">
         <v>78</v>
       </c>
-      <c r="F70" s="89">
+      <c r="F70" s="90">
         <f>VLOOKUP($F$68,$A$68:$D$71,3,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="G70" s="89"/>
+      <c r="G70" s="90"/>
     </row>
     <row r="71" spans="1:15">
-      <c r="A71" s="83">
+      <c r="A71" s="48">
         <v>103</v>
       </c>
-      <c r="B71" s="83" t="s">
+      <c r="B71" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="83">
+      <c r="C71" s="48">
         <v>19</v>
       </c>
-      <c r="D71" s="83">
+      <c r="D71" s="48">
         <v>92</v>
       </c>
-      <c r="F71" s="54">
+      <c r="F71" s="76">
         <f>VLOOKUP($F$68,$A$68:$D$71,4,FALSE)</f>
         <v>92</v>
       </c>
-      <c r="G71" s="54"/>
+      <c r="G71" s="76"/>
     </row>
     <row r="74" spans="1:15">
-      <c r="F74" s="91"/>
-      <c r="G74" s="91"/>
+      <c r="F74" s="87"/>
+      <c r="G74" s="87"/>
     </row>
     <row r="75" spans="1:15">
-      <c r="F75" s="91"/>
-      <c r="G75" s="91"/>
+      <c r="F75" s="87"/>
+      <c r="G75" s="87"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="F76" s="91"/>
-      <c r="G76" s="91"/>
+      <c r="F76" s="87"/>
+      <c r="G76" s="87"/>
     </row>
     <row r="77" spans="1:15">
-      <c r="F77" s="91"/>
-      <c r="G77" s="91"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="87"/>
     </row>
     <row r="78" spans="1:15">
-      <c r="F78" s="92"/>
-      <c r="G78" s="92"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="53"/>
     </row>
   </sheetData>
   <autoFilter ref="A38:I58" xr:uid="{35914A46-0205-471D-B2D7-66681A3205BE}">
@@ -11105,6 +12474,16 @@
     </sortState>
   </autoFilter>
   <mergeCells count="18">
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="L38:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
     <mergeCell ref="F75:G75"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F77:G77"/>
@@ -11113,16 +12492,6 @@
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F74:G74"/>
-    <mergeCell ref="L38:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="M48:N48"/>
   </mergeCells>
   <conditionalFormatting sqref="M47:N47">
     <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
@@ -11200,4 +12569,250 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AF317E-9EAE-490E-A6DA-3381FFA4FB86}">
+  <dimension ref="D4:I24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="4" spans="4:9">
+      <c r="D4" s="93"/>
+    </row>
+    <row r="5" spans="4:9">
+      <c r="D5" s="93"/>
+    </row>
+    <row r="6" spans="4:9">
+      <c r="D6" s="93"/>
+    </row>
+    <row r="7" spans="4:9">
+      <c r="D7" s="93"/>
+    </row>
+    <row r="8" spans="4:9">
+      <c r="D8" s="93"/>
+    </row>
+    <row r="15" spans="4:9">
+      <c r="I15" s="95">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9">
+      <c r="I16" s="95">
+        <f>1-I15</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9">
+      <c r="I17" s="94"/>
+    </row>
+    <row r="18" spans="6:9">
+      <c r="F18" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="94"/>
+    </row>
+    <row r="19" spans="6:9">
+      <c r="F19" s="38"/>
+      <c r="G19" s="92" t="s">
+        <v>197</v>
+      </c>
+      <c r="H19" s="92"/>
+      <c r="I19" s="95"/>
+    </row>
+    <row r="20" spans="6:9">
+      <c r="F20" s="38"/>
+      <c r="G20" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="H20" s="92"/>
+    </row>
+    <row r="21" spans="6:9">
+      <c r="F21" s="38"/>
+      <c r="G21" s="92" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="92"/>
+    </row>
+    <row r="22" spans="6:9">
+      <c r="F22" s="38"/>
+      <c r="G22" s="92" t="s">
+        <v>200</v>
+      </c>
+      <c r="H22" s="92"/>
+    </row>
+    <row r="23" spans="6:9">
+      <c r="F23" s="38"/>
+      <c r="G23" s="92" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="92"/>
+    </row>
+    <row r="24" spans="6:9">
+      <c r="F24" s="38"/>
+      <c r="G24" s="92" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+  </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3073" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3074" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3075" r:id="rId6" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3076" r:id="rId7" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3077" r:id="rId8" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3078" r:id="rId9" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
understan check box , how to hide the colums undestand conditional rols do a progress bar
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B671ED8C-7F6E-4E48-9CB6-1CD9EADFD4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB38B495-CE00-4138-8744-336AF49F3C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
   <si>
     <t>Day</t>
   </si>
@@ -1316,29 +1316,53 @@
     <t>TO DO LIST</t>
   </si>
   <si>
-    <t>STEP 1</t>
-  </si>
-  <si>
-    <t>STEP 2</t>
-  </si>
-  <si>
-    <t>STEP 3</t>
-  </si>
-  <si>
-    <t>STEP 4</t>
-  </si>
-  <si>
-    <t>STEP 5</t>
-  </si>
-  <si>
-    <t>STEP 6</t>
+    <t>TASK 1</t>
+  </si>
+  <si>
+    <t>TASK 2</t>
+  </si>
+  <si>
+    <t>TASK 3</t>
+  </si>
+  <si>
+    <t>TASK 4</t>
+  </si>
+  <si>
+    <t>TASK 5</t>
+  </si>
+  <si>
+    <t>TASK 6</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Tl5SRQ_yduw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check box </t>
+  </si>
+  <si>
+    <t>task1</t>
+  </si>
+  <si>
+    <t>task2</t>
+  </si>
+  <si>
+    <t>task3</t>
+  </si>
+  <si>
+    <t>task4</t>
+  </si>
+  <si>
+    <t>task5</t>
+  </si>
+  <si>
+    <t>task6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1488,13 +1512,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1585,6 +1604,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1650,7 +1675,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1775,11 +1800,26 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1865,9 +1905,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1892,19 +1929,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3659,6 +3718,278 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tasks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-CD83-4BC7-BEDD-5096ABC08B3C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CD83-4BC7-BEDD-5096ABC08B3C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>PROGRESS!$F$28:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD83-4BC7-BEDD-5096ABC08B3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3690,17 +4021,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.26680387797131411"/>
-          <c:y val="0.14975915221579963"/>
-          <c:w val="0.44059530003039266"/>
-          <c:h val="0.65816417095261937"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:doughnutChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -3738,22 +4059,22 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>PROGRESS!$I$15:$I$16</c:f>
+              <c:f>PROGRESS!$L$26:$L$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.35</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D0E0-4A92-8752-BFD7476E78FE}"/>
+              <c16:uniqueId val="{00000000-47C5-44C5-8387-4E2862194BAD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4049,6 +4370,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6051,6 +6412,607 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6570,27 +7532,51 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$19" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$24" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$16" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$O$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6613,7 +7599,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D373FC-6A76-4EF5-8EDA-FB3FA40FE4E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6651,7 +7637,7 @@
             <xdr:cNvPr id="5" name="Region">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A93A7A-4F28-44F6-B1C3-EE92BC30ECC6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6727,7 +7713,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDBFBFC-974C-4F40-8C16-82AA0EC6FE0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6763,7 +7749,7 @@
         <xdr:cNvPr id="3" name="Connector: Elbow 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73FDCF07-CE3B-4720-B44D-333D681B66E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6818,7 +7804,7 @@
         <xdr:cNvPr id="11" name="Arrow: Right 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12FEF473-6494-4D20-891F-174955B9799E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6883,7 +7869,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{008B365B-7A5A-443B-A463-C6AA6489F945}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6921,7 +7907,7 @@
             <xdr:cNvPr id="3" name="Grade">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E01742-5E80-41B4-8904-EE854865C018}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6999,7 +7985,7 @@
             <xdr:cNvPr id="4" name="Age">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C491AF-540D-4898-8A91-39CE790CE12B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7077,7 +8063,7 @@
             <xdr:cNvPr id="5" name="Fees Paid">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{440F3CC9-3086-4C5E-92B9-0A14DA28397C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7153,7 +8139,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459502CA-70D3-4C34-95B8-D7EF7FE2BCD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7176,56 +8162,20 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>250371</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3153B70-10DB-499D-A906-479E3C478A65}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>446049</xdr:colOff>
+          <xdr:colOff>449580</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>178420</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7281,14 +8231,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3074" name="Check Box 2" hidden="1">
@@ -7297,7 +8252,7 @@
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52086989-7903-423A-8308-1DE0FBEB5216}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7337,20 +8292,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3075" name="Check Box 3" hidden="1">
@@ -7359,7 +8319,7 @@
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A75F294-67BE-498D-A644-B89B1BE72414}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7399,20 +8359,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3076" name="Check Box 4" hidden="1">
@@ -7421,7 +8386,7 @@
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BCBF4C5-62A1-4B19-94B7-22DE0C4FCC1C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7461,20 +8426,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3077" name="Check Box 5" hidden="1">
@@ -7483,7 +8453,7 @@
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5038C94-8BE6-4168-80F0-422D6C3657DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7523,20 +8493,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>226740</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>3718</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="219309" cy="174702"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3078" name="Check Box 6" hidden="1">
@@ -7545,7 +8520,7 @@
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45F8994-423C-47ED-BF58-3A9AECBDBD5E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7585,10 +8560,484 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3080" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3080"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3081" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3081"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3082" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3082"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3083" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3083"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3084" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3084"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>182880</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>426720</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3085" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3085"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD0F59C0-A144-46CE-9C4E-BC8D60E68671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8977,10 +10426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D52DEAC-DA9C-4AAE-B79E-917F758942A1}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9025,13 +10474,13 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" ht="60.6" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -9118,15 +10567,28 @@
         <v>34</v>
       </c>
     </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="62"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="F2:J2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{CA270109-D5D8-4121-BB2A-2843914E30D2}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{B5A4BBC4-EDC5-40C1-99D5-EDA50CB05374}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9149,44 +10611,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -9198,22 +10660,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="72"/>
-      <c r="H7" s="61" t="s">
+      <c r="G7" s="79"/>
+      <c r="H7" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61" t="s">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61" t="s">
+      <c r="K7" s="68"/>
+      <c r="L7" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="61"/>
+      <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -9226,26 +10688,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="69">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62">
+      <c r="G8" s="69"/>
+      <c r="H8" s="69">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62">
+      <c r="I8" s="69"/>
+      <c r="J8" s="69">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62">
+      <c r="K8" s="69"/>
+      <c r="L8" s="69">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="62"/>
+      <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -9258,14 +10720,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -9278,14 +10740,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -9340,10 +10802,10 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F14" s="65" t="s">
+      <c r="F14" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="65"/>
+      <c r="G14" s="72"/>
       <c r="K14" s="15" t="s">
         <v>66</v>
       </c>
@@ -9526,15 +10988,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="10" t="s">
@@ -9568,14 +11030,14 @@
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="68" t="s">
+      <c r="F34" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="68"/>
-      <c r="J34" s="68" t="s">
+      <c r="G34" s="75"/>
+      <c r="J34" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="68"/>
+      <c r="K34" s="75"/>
       <c r="M34" s="14" t="s">
         <v>86</v>
       </c>
@@ -9747,10 +11209,10 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="64" t="s">
+      <c r="I42" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="64"/>
+      <c r="J42" s="71"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
@@ -9866,11 +11328,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.6">
-      <c r="B57" s="63" t="s">
+      <c r="B57" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="17"/>
       <c r="H57">
         <v>123</v>
@@ -9880,9 +11342,9 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
+      <c r="B58" s="70"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="70"/>
       <c r="E58" s="17"/>
       <c r="H58">
         <v>124</v>
@@ -9900,11 +11362,11 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="69" t="s">
+      <c r="B60" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="69"/>
-      <c r="D60" s="69"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
       <c r="H60">
         <v>126</v>
       </c>
@@ -9916,10 +11378,10 @@
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="70" t="s">
+      <c r="C61" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="71"/>
+      <c r="D61" s="78"/>
       <c r="H61">
         <v>127</v>
       </c>
@@ -9931,10 +11393,10 @@
       <c r="B62" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="74"/>
+      <c r="D62" s="81"/>
       <c r="H62">
         <v>128</v>
       </c>
@@ -9946,10 +11408,10 @@
       <c r="B63" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="74"/>
+      <c r="D63" s="81"/>
       <c r="H63">
         <v>129</v>
       </c>
@@ -9961,10 +11423,10 @@
       <c r="B64" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="73" t="s">
+      <c r="C64" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="74"/>
+      <c r="D64" s="81"/>
       <c r="H64">
         <v>130</v>
       </c>
@@ -9989,10 +11451,10 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="B67" s="75" t="s">
+      <c r="B67" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="75"/>
+      <c r="C67" s="82"/>
       <c r="D67" s="9">
         <v>34</v>
       </c>
@@ -10004,10 +11466,10 @@
       </c>
     </row>
     <row r="68" spans="2:10">
-      <c r="B68" s="75" t="s">
+      <c r="B68" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="75"/>
+      <c r="C68" s="82"/>
       <c r="D68" s="9">
         <v>35</v>
       </c>
@@ -10019,10 +11481,10 @@
       </c>
     </row>
     <row r="69" spans="2:10">
-      <c r="B69" s="75" t="s">
+      <c r="B69" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="75"/>
+      <c r="C69" s="82"/>
       <c r="D69" s="9">
         <v>36</v>
       </c>
@@ -10037,10 +11499,10 @@
       </c>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="75" t="s">
+      <c r="B70" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="C70" s="75"/>
+      <c r="C70" s="82"/>
       <c r="D70" s="9">
         <v>37</v>
       </c>
@@ -10052,10 +11514,10 @@
       </c>
     </row>
     <row r="71" spans="2:10">
-      <c r="B71" s="75" t="s">
+      <c r="B71" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="C71" s="75"/>
+      <c r="C71" s="82"/>
       <c r="D71" s="9">
         <v>38</v>
       </c>
@@ -10067,10 +11529,10 @@
       </c>
     </row>
     <row r="72" spans="2:10">
-      <c r="B72" s="75" t="s">
+      <c r="B72" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="75"/>
+      <c r="C72" s="82"/>
       <c r="D72" s="9">
         <v>39</v>
       </c>
@@ -10082,10 +11544,10 @@
       </c>
     </row>
     <row r="73" spans="2:10">
-      <c r="B73" s="75" t="s">
+      <c r="B73" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="75"/>
+      <c r="C73" s="82"/>
       <c r="D73" s="9">
         <v>40</v>
       </c>
@@ -10137,18 +11599,18 @@
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="56"/>
-      <c r="D81" s="56"/>
-      <c r="E81" s="56"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="56"/>
-      <c r="C82" s="56"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="63"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="63"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="10" t="s">
@@ -10239,18 +11701,18 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="57" t="s">
+      <c r="B97" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="57"/>
-      <c r="D97" s="57"/>
-      <c r="E97" s="57"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="57"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="57"/>
-      <c r="E98" s="57"/>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="10" t="s">
@@ -10341,22 +11803,22 @@
       </c>
     </row>
     <row r="114" spans="2:14">
-      <c r="B114" s="58" t="s">
+      <c r="B114" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="58"/>
-      <c r="D114" s="58"/>
-      <c r="E114" s="58"/>
-      <c r="F114" s="58"/>
-      <c r="G114" s="58"/>
+      <c r="C114" s="65"/>
+      <c r="D114" s="65"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="65"/>
     </row>
     <row r="115" spans="2:14">
-      <c r="B115" s="58"/>
-      <c r="C115" s="58"/>
-      <c r="D115" s="58"/>
-      <c r="E115" s="58"/>
-      <c r="F115" s="58"/>
-      <c r="G115" s="58"/>
+      <c r="B115" s="65"/>
+      <c r="C115" s="65"/>
+      <c r="D115" s="65"/>
+      <c r="E115" s="65"/>
+      <c r="F115" s="65"/>
+      <c r="G115" s="65"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="10" t="s">
@@ -10461,11 +11923,11 @@
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="L120" s="77" t="s">
+      <c r="L120" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="M120" s="78"/>
-      <c r="N120" s="78"/>
+      <c r="M120" s="85"/>
+      <c r="N120" s="85"/>
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="3" t="s">
@@ -10488,9 +11950,9 @@
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="L121" s="78"/>
-      <c r="M121" s="78"/>
-      <c r="N121" s="78"/>
+      <c r="L121" s="85"/>
+      <c r="M121" s="85"/>
+      <c r="N121" s="85"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="3" t="s">
@@ -10513,10 +11975,10 @@
       <c r="D123" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J123" s="76" t="s">
+      <c r="J123" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="K123" s="76"/>
+      <c r="K123" s="83"/>
       <c r="L123" s="21" t="str" cm="1">
         <f t="array" ref="L123:L125">_xlfn.UNIQUE(B118:B127)</f>
         <v>Laptop</v>
@@ -10573,20 +12035,20 @@
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="57" t="s">
+      <c r="B130" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="57"/>
-      <c r="D130" s="57"/>
-      <c r="E130" s="57"/>
-      <c r="F130" s="57"/>
+      <c r="C130" s="64"/>
+      <c r="D130" s="64"/>
+      <c r="E130" s="64"/>
+      <c r="F130" s="64"/>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" s="57"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="57"/>
-      <c r="E131" s="57"/>
-      <c r="F131" s="57"/>
+      <c r="B131" s="64"/>
+      <c r="C131" s="64"/>
+      <c r="D131" s="64"/>
+      <c r="E131" s="64"/>
+      <c r="F131" s="64"/>
     </row>
     <row r="133" spans="2:11">
       <c r="B133" s="10" t="s">
@@ -10631,10 +12093,10 @@
       <c r="I135" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="J135" s="79" t="s">
+      <c r="J135" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="80"/>
+      <c r="K135" s="87"/>
     </row>
     <row r="136" spans="2:11">
       <c r="B136" s="3" t="s">
@@ -10650,11 +12112,11 @@
       <c r="I136" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J136" s="79">
+      <c r="J136" s="86">
         <f>IFERROR(VLOOKUP($J$135,$B$134:$D$143,2,FALSE),"Not found")</f>
         <v>300</v>
       </c>
-      <c r="K136" s="80"/>
+      <c r="K136" s="87"/>
     </row>
     <row r="137" spans="2:11">
       <c r="B137" s="3" t="s">
@@ -10753,10 +12215,10 @@
       <c r="E146" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="81" t="s">
+      <c r="G146" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="H146" s="82"/>
+      <c r="H146" s="89"/>
     </row>
     <row r="147" spans="2:10" ht="16.8" customHeight="1">
       <c r="B147" s="3" t="s">
@@ -10771,14 +12233,14 @@
       <c r="E147" s="3">
         <v>85</v>
       </c>
-      <c r="G147" s="84" t="s">
+      <c r="G147" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="H147" s="84"/>
-      <c r="I147" s="85" t="s">
+      <c r="H147" s="62"/>
+      <c r="I147" s="91" t="s">
         <v>138</v>
       </c>
-      <c r="J147" s="85"/>
+      <c r="J147" s="91"/>
     </row>
     <row r="148" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B148" s="3" t="s">
@@ -10793,11 +12255,11 @@
       <c r="E148" s="3">
         <v>78</v>
       </c>
-      <c r="I148" s="86" t="str">
+      <c r="I148" s="92" t="str">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,2,FALSE),"NOT FOUND")</f>
         <v>charlie@email.com</v>
       </c>
-      <c r="J148" s="86"/>
+      <c r="J148" s="92"/>
     </row>
     <row r="149" spans="2:10" ht="22.2" customHeight="1">
       <c r="B149" s="3" t="s">
@@ -10812,11 +12274,11 @@
       <c r="E149" s="3">
         <v>92</v>
       </c>
-      <c r="I149" s="86">
+      <c r="I149" s="92">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,3,FALSE),"NOT FOUND")</f>
         <v>7654321098</v>
       </c>
-      <c r="J149" s="86"/>
+      <c r="J149" s="92"/>
     </row>
     <row r="150" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B150" s="3" t="s">
@@ -10831,11 +12293,11 @@
       <c r="E150" s="3">
         <v>67</v>
       </c>
-      <c r="I150" s="86">
+      <c r="I150" s="92">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,4,FALSE),"NOT FOUND")</f>
         <v>92</v>
       </c>
-      <c r="J150" s="86"/>
+      <c r="J150" s="92"/>
     </row>
     <row r="151" spans="2:10" ht="21.6" customHeight="1">
       <c r="B151" s="3" t="s">
@@ -10850,8 +12312,8 @@
       <c r="E151" s="3">
         <v>74</v>
       </c>
-      <c r="I151" s="83"/>
-      <c r="J151" s="83"/>
+      <c r="I151" s="90"/>
+      <c r="J151" s="90"/>
     </row>
     <row r="152" spans="2:10" ht="21.6" customHeight="1"/>
   </sheetData>
@@ -10906,12 +12368,12 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="C8:C27">
-    <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="31" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D27">
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="greaterThan">
       <formula>"PASS"</formula>
     </cfRule>
     <cfRule type="iconSet" priority="29">
@@ -10923,10 +12385,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:D73">
-    <cfRule type="cellIs" dxfId="15" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
       <formula>37</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="27" operator="between">
       <formula>34</formula>
       <formula>38</formula>
     </cfRule>
@@ -10987,18 +12449,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:C95">
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="lessThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:C110">
-    <cfRule type="top10" dxfId="12" priority="17" rank="5"/>
+    <cfRule type="top10" dxfId="14" priority="17" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C134:C143">
-    <cfRule type="top10" dxfId="11" priority="5" rank="5"/>
+    <cfRule type="top10" dxfId="13" priority="5" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>AND(C134&gt;500,D134="North")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11404,11 +12866,11 @@
       <c r="J38" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="91" t="s">
+      <c r="L38" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="M38" s="91"/>
-      <c r="N38" s="91"/>
+      <c r="M38" s="97"/>
+      <c r="N38" s="97"/>
       <c r="R38" s="14" t="s">
         <v>86</v>
       </c>
@@ -11454,9 +12916,9 @@
         <f>IF(AND(G39&gt;70,I39="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L39" s="91"/>
-      <c r="M39" s="91"/>
-      <c r="N39" s="91"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="97"/>
       <c r="R39" s="47">
         <v>104</v>
       </c>
@@ -11502,11 +12964,11 @@
         <f t="shared" ref="J40:J58" si="0">IF(AND(G40&gt;70,I40="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L40" s="92" t="s">
+      <c r="L40" s="98" t="s">
         <v>194</v>
       </c>
-      <c r="M40" s="92"/>
-      <c r="N40" s="92"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
       <c r="R40" s="47">
         <v>108</v>
       </c>
@@ -11555,11 +13017,11 @@
       <c r="L41" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="M41" s="92">
+      <c r="M41" s="98">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,2,FALSE),"Not found")</f>
         <v>22</v>
       </c>
-      <c r="N41" s="92"/>
+      <c r="N41" s="98"/>
       <c r="R41" s="47">
         <v>112</v>
       </c>
@@ -11608,11 +13070,11 @@
       <c r="L42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="92" t="str">
+      <c r="M42" s="98" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,3,FALSE),"Not found")</f>
         <v>david@email.com</v>
       </c>
-      <c r="N42" s="92"/>
+      <c r="N42" s="98"/>
       <c r="R42" s="47">
         <v>120</v>
       </c>
@@ -11661,11 +13123,11 @@
       <c r="L43" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="92">
+      <c r="M43" s="98">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,4,FALSE),"Not found")</f>
         <v>6543210987</v>
       </c>
-      <c r="N43" s="92"/>
+      <c r="N43" s="98"/>
       <c r="R43" s="47" t="s">
         <v>87</v>
       </c>
@@ -11714,11 +13176,11 @@
       <c r="L44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M44" s="92">
+      <c r="M44" s="98">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,5,FALSE),"Not found")</f>
         <v>11</v>
       </c>
-      <c r="N44" s="92"/>
+      <c r="N44" s="98"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="37">
@@ -11755,11 +13217,11 @@
       <c r="L45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="92">
+      <c r="M45" s="98">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,6,FALSE),"Not found")</f>
         <v>67</v>
       </c>
-      <c r="N45" s="92"/>
+      <c r="N45" s="98"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="37">
@@ -11796,11 +13258,11 @@
       <c r="L46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="M46" s="92">
+      <c r="M46" s="98">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,7,FALSE),"Not found")</f>
         <v>85</v>
       </c>
-      <c r="N46" s="92"/>
+      <c r="N46" s="98"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="37">
@@ -11837,11 +13299,11 @@
       <c r="L47" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="92" t="str">
+      <c r="M47" s="98" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,8,FALSE),"Not found")</f>
         <v>No</v>
       </c>
-      <c r="N47" s="92"/>
+      <c r="N47" s="98"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="37">
@@ -11875,8 +13337,8 @@
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="M48" s="83"/>
-      <c r="N48" s="83"/>
+      <c r="M48" s="90"/>
+      <c r="N48" s="90"/>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="37">
@@ -12379,10 +13841,10 @@
       <c r="D68" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="88">
+      <c r="F68" s="94">
         <v>103</v>
       </c>
-      <c r="G68" s="88"/>
+      <c r="G68" s="94"/>
       <c r="N68" s="44">
         <v>92</v>
       </c>
@@ -12400,11 +13862,11 @@
       <c r="D69" s="48">
         <v>85</v>
       </c>
-      <c r="F69" s="89" t="str">
+      <c r="F69" s="95" t="str">
         <f>VLOOKUP($F$68,$A$68:$D$71,2,FALSE)</f>
         <v>Charlie</v>
       </c>
-      <c r="G69" s="89"/>
+      <c r="G69" s="95"/>
       <c r="N69" s="44">
         <v>95</v>
       </c>
@@ -12422,11 +13884,11 @@
       <c r="D70" s="48">
         <v>78</v>
       </c>
-      <c r="F70" s="90">
+      <c r="F70" s="96">
         <f>VLOOKUP($F$68,$A$68:$D$71,3,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="G70" s="90"/>
+      <c r="G70" s="96"/>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" s="48">
@@ -12441,27 +13903,27 @@
       <c r="D71" s="48">
         <v>92</v>
       </c>
-      <c r="F71" s="76">
+      <c r="F71" s="83">
         <f>VLOOKUP($F$68,$A$68:$D$71,4,FALSE)</f>
         <v>92</v>
       </c>
-      <c r="G71" s="76"/>
+      <c r="G71" s="83"/>
     </row>
     <row r="74" spans="1:15">
-      <c r="F74" s="87"/>
-      <c r="G74" s="87"/>
+      <c r="F74" s="93"/>
+      <c r="G74" s="93"/>
     </row>
     <row r="75" spans="1:15">
-      <c r="F75" s="87"/>
-      <c r="G75" s="87"/>
+      <c r="F75" s="93"/>
+      <c r="G75" s="93"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="F76" s="87"/>
-      <c r="G76" s="87"/>
+      <c r="F76" s="93"/>
+      <c r="G76" s="93"/>
     </row>
     <row r="77" spans="1:15">
-      <c r="F77" s="87"/>
-      <c r="G77" s="87"/>
+      <c r="F77" s="93"/>
+      <c r="G77" s="93"/>
     </row>
     <row r="78" spans="1:15">
       <c r="F78" s="53"/>
@@ -12494,20 +13956,20 @@
     <mergeCell ref="F74:G74"/>
   </mergeCells>
   <conditionalFormatting sqref="M47:N47">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:N46">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">
       <formula>75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I58">
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",I39)))</formula>
     </cfRule>
     <cfRule type="iconSet" priority="6">
@@ -12573,96 +14035,209 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AF317E-9EAE-490E-A6DA-3381FFA4FB86}">
-  <dimension ref="D4:I24"/>
+  <dimension ref="D4:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="9" max="9" width="26.5546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:9">
-      <c r="D4" s="93"/>
-    </row>
-    <row r="5" spans="4:9">
-      <c r="D5" s="93"/>
-    </row>
-    <row r="6" spans="4:9">
-      <c r="D6" s="93"/>
-    </row>
-    <row r="7" spans="4:9">
-      <c r="D7" s="93"/>
-    </row>
-    <row r="8" spans="4:9">
-      <c r="D8" s="93"/>
-    </row>
-    <row r="15" spans="4:9">
-      <c r="I15" s="95">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="16" spans="4:9">
-      <c r="I16" s="95">
-        <f>1-I15</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9">
-      <c r="I17" s="94"/>
-    </row>
-    <row r="18" spans="6:9">
-      <c r="F18" s="96" t="s">
+    <row r="4" spans="4:15">
+      <c r="D4" s="54"/>
+    </row>
+    <row r="5" spans="4:15">
+      <c r="D5" s="54"/>
+    </row>
+    <row r="6" spans="4:15">
+      <c r="D6" s="54"/>
+    </row>
+    <row r="7" spans="4:15">
+      <c r="D7" s="54"/>
+    </row>
+    <row r="8" spans="4:15">
+      <c r="D8" s="54"/>
+    </row>
+    <row r="15" spans="4:15">
+      <c r="I15" s="56"/>
+      <c r="L15" s="101" t="s">
+        <v>205</v>
+      </c>
+      <c r="M15" s="102"/>
+      <c r="N15" s="9"/>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:15">
+      <c r="I16" s="99"/>
+      <c r="J16" s="99"/>
+      <c r="L16" s="98" t="s">
+        <v>206</v>
+      </c>
+      <c r="M16" s="98"/>
+      <c r="N16" s="9"/>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15">
+      <c r="I17" s="55"/>
+      <c r="L17" s="98" t="s">
+        <v>207</v>
+      </c>
+      <c r="M17" s="98"/>
+      <c r="N17" s="9"/>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15">
+      <c r="F18" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="94"/>
-    </row>
-    <row r="19" spans="6:9">
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="55"/>
+      <c r="L18" s="98" t="s">
+        <v>208</v>
+      </c>
+      <c r="M18" s="98"/>
+      <c r="N18" s="9"/>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15">
       <c r="F19" s="38"/>
-      <c r="G19" s="92" t="s">
+      <c r="G19" s="98" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="92"/>
-      <c r="I19" s="95"/>
-    </row>
-    <row r="20" spans="6:9">
+      <c r="H19" s="98"/>
+      <c r="I19" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="98" t="s">
+        <v>209</v>
+      </c>
+      <c r="M19" s="98"/>
+      <c r="N19" s="9"/>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15">
       <c r="F20" s="38"/>
-      <c r="G20" s="92" t="s">
+      <c r="G20" s="98" t="s">
         <v>198</v>
       </c>
-      <c r="H20" s="92"/>
-    </row>
-    <row r="21" spans="6:9">
+      <c r="H20" s="98"/>
+      <c r="I20" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="98" t="s">
+        <v>210</v>
+      </c>
+      <c r="M20" s="98"/>
+      <c r="N20" s="9"/>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15">
       <c r="F21" s="38"/>
-      <c r="G21" s="92" t="s">
+      <c r="G21" s="98" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="92"/>
-    </row>
-    <row r="22" spans="6:9">
+      <c r="H21" s="98"/>
+      <c r="I21" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15">
       <c r="F22" s="38"/>
-      <c r="G22" s="92" t="s">
+      <c r="G22" s="98" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="92"/>
-    </row>
-    <row r="23" spans="6:9">
+      <c r="H22" s="98"/>
+      <c r="I22" s="56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="6:15">
       <c r="F23" s="38"/>
-      <c r="G23" s="92" t="s">
+      <c r="G23" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="H23" s="92"/>
-    </row>
-    <row r="24" spans="6:9">
+      <c r="H23" s="98"/>
+      <c r="I23" s="56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:15">
       <c r="F24" s="38"/>
-      <c r="G24" s="92" t="s">
+      <c r="G24" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="H24" s="92"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>COUNTA(O15:O20)</f>
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <f>COUNTIF(O15:O20,TRUE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="6:15">
+      <c r="I25" s="99">
+        <f>COUNTIF(I19:I24,TRUE)/COUNTA(G19:H24)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J25" s="99"/>
+    </row>
+    <row r="26" spans="6:15">
+      <c r="I26" s="57">
+        <f>1-I25</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="L26" s="103">
+        <f>M24/L24</f>
+        <v>1</v>
+      </c>
+      <c r="M26" s="103"/>
+      <c r="N26" s="103"/>
+    </row>
+    <row r="27" spans="6:15">
+      <c r="L27" s="104">
+        <f>1-L26</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="104"/>
+      <c r="N27" s="104"/>
+    </row>
+    <row r="28" spans="6:15">
+      <c r="F28" s="55">
+        <f>COUNTIF(I19:I24,TRUE)/COUNTA(G19:H24)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="6:15">
+      <c r="F29" s="55">
+        <f>1-F28</f>
+        <v>0.33333333333333337</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="15">
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="G19:H19"/>
@@ -12670,8 +14245,66 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{35AB654F-8FEC-4257-98E5-B2F6483F98EC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:J16">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8CA93CD3-5C7A-47BC-B69B-73AB760619A0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15:M20">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>$O15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>$O$15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26:L27">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{907DDA4C-9B31-47B8-9B45-E5CAF8362399}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12811,8 +14444,189 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3080" r:id="rId10" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3081" r:id="rId11" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3082" r:id="rId12" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3083" r:id="rId13" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3084" r:id="rId14" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3085" r:id="rId15" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>182880</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>426720</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{35AB654F-8FEC-4257-98E5-B2F6483F98EC}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8CA93CD3-5C7A-47BC-B69B-73AB760619A0}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I16:J16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{907DDA4C-9B31-47B8-9B45-E5CAF8362399}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L26:L27</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
learn vlookup, vlookup is only F to R
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB38B495-CE00-4138-8744-336AF49F3C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8523D685-8899-42C5-AEF3-4381576C01D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="2712" yWindow="0" windowWidth="17280" windowHeight="9420" activeTab="4" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
     <sheet name="PHASE1" sheetId="2" r:id="rId2"/>
     <sheet name="VIEW STUDENTS" sheetId="3" r:id="rId3"/>
     <sheet name="PROGRESS" sheetId="4" r:id="rId4"/>
+    <sheet name="PHASE 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PHASE1!$B$32:$D$52</definedName>
@@ -29,17 +30,17 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId8"/>
         <x14:slicerCache r:id="rId9"/>
         <x14:slicerCache r:id="rId10"/>
         <x14:slicerCache r:id="rId11"/>
+        <x14:slicerCache r:id="rId12"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="232">
   <si>
     <t>Day</t>
   </si>
@@ -1357,12 +1358,131 @@
   <si>
     <t>task6</t>
   </si>
+  <si>
+    <t>1️⃣ VLOOKUP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🔹 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What is this?</t>
+    </r>
+  </si>
+  <si>
+    <t>VLOOKUP finds data in a column and returns a value from another column.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🔹 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Why use this?</t>
+    </r>
+  </si>
+  <si>
+    <t>To quickly find and match data in a large table.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🔹 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When use this?</t>
+    </r>
+  </si>
+  <si>
+    <t>When you need to find a price, employee name, or any data using a key (like an ID).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🔹 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How to use this?</t>
+    </r>
+  </si>
+  <si>
+    <t>Formula:</t>
+  </si>
+  <si>
+    <t>📌 Example: Find a salary using an employee ID.</t>
+  </si>
+  <si>
+    <t>"=VLOOKUP(lookup_value, table_range, column_number, FALSE)"</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>find by ID</t>
+  </si>
+  <si>
+    <t>📝 Practical 1: Find Employee Salary by ID</t>
+  </si>
+  <si>
+    <t>📝 Practical 2: Find Product Price by Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>find by Name</t>
+  </si>
+  <si>
+    <t>VLOOKUP cannot search backward (it only looks from left to right).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1507,6 +1627,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1670,12 +1814,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1806,6 +1951,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1821,6 +1968,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1835,12 +2030,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1869,47 +2058,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1923,16 +2076,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1941,10 +2088,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -4041,6 +4205,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C9CE-489F-A94B-5303C395E811}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4056,6 +4225,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C9CE-489F-A94B-5303C395E811}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -9020,7 +9194,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD0F59C0-A144-46CE-9C4E-BC8D60E68671}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10429,7 +10603,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10474,13 +10648,13 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="60.6" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -10568,14 +10742,14 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="61" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10594,6 +10768,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB262F42-5A31-4E7C-9BC0-8AA576C134EE}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:N152"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A145" workbookViewId="0">
@@ -10611,44 +10788,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -10660,22 +10837,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="68" t="s">
+      <c r="G7" s="80"/>
+      <c r="H7" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68" t="s">
+      <c r="I7" s="79"/>
+      <c r="J7" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68" t="s">
+      <c r="K7" s="79"/>
+      <c r="L7" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="68"/>
+      <c r="M7" s="79"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -10688,26 +10865,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F8" s="78">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69">
+      <c r="G8" s="78"/>
+      <c r="H8" s="78">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69">
+      <c r="I8" s="78"/>
+      <c r="J8" s="78">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69">
+      <c r="K8" s="78"/>
+      <c r="L8" s="78">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="69"/>
+      <c r="M8" s="78"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -10720,14 +10897,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -10740,14 +10917,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -10802,10 +10979,10 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="72"/>
+      <c r="G14" s="88"/>
       <c r="K14" s="15" t="s">
         <v>66</v>
       </c>
@@ -10988,15 +11165,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="10" t="s">
@@ -11030,14 +11207,14 @@
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="75" t="s">
+      <c r="F34" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="J34" s="75" t="s">
+      <c r="G34" s="91"/>
+      <c r="J34" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="75"/>
+      <c r="K34" s="91"/>
       <c r="M34" s="14" t="s">
         <v>86</v>
       </c>
@@ -11209,10 +11386,10 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="71" t="s">
+      <c r="I42" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="71"/>
+      <c r="J42" s="87"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
@@ -11328,11 +11505,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.6">
-      <c r="B57" s="70" t="s">
+      <c r="B57" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="70"/>
-      <c r="D57" s="70"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="86"/>
       <c r="E57" s="17"/>
       <c r="H57">
         <v>123</v>
@@ -11342,9 +11519,9 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="70"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
+      <c r="B58" s="86"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="86"/>
       <c r="E58" s="17"/>
       <c r="H58">
         <v>124</v>
@@ -11362,11 +11539,11 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="76" t="s">
+      <c r="B60" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
+      <c r="C60" s="92"/>
+      <c r="D60" s="92"/>
       <c r="H60">
         <v>126</v>
       </c>
@@ -11378,10 +11555,10 @@
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="77" t="s">
+      <c r="C61" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="78"/>
+      <c r="D61" s="94"/>
       <c r="H61">
         <v>127</v>
       </c>
@@ -11393,10 +11570,10 @@
       <c r="B62" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="80" t="s">
+      <c r="C62" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="81"/>
+      <c r="D62" s="76"/>
       <c r="H62">
         <v>128</v>
       </c>
@@ -11408,10 +11585,10 @@
       <c r="B63" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="81"/>
+      <c r="D63" s="76"/>
       <c r="H63">
         <v>129</v>
       </c>
@@ -11423,10 +11600,10 @@
       <c r="B64" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="80" t="s">
+      <c r="C64" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="81"/>
+      <c r="D64" s="76"/>
       <c r="H64">
         <v>130</v>
       </c>
@@ -11451,10 +11628,10 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="B67" s="82" t="s">
+      <c r="B67" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="82"/>
+      <c r="C67" s="77"/>
       <c r="D67" s="9">
         <v>34</v>
       </c>
@@ -11466,10 +11643,10 @@
       </c>
     </row>
     <row r="68" spans="2:10">
-      <c r="B68" s="82" t="s">
+      <c r="B68" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="82"/>
+      <c r="C68" s="77"/>
       <c r="D68" s="9">
         <v>35</v>
       </c>
@@ -11481,10 +11658,10 @@
       </c>
     </row>
     <row r="69" spans="2:10">
-      <c r="B69" s="82" t="s">
+      <c r="B69" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="82"/>
+      <c r="C69" s="77"/>
       <c r="D69" s="9">
         <v>36</v>
       </c>
@@ -11499,10 +11676,10 @@
       </c>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="82" t="s">
+      <c r="B70" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="C70" s="82"/>
+      <c r="C70" s="77"/>
       <c r="D70" s="9">
         <v>37</v>
       </c>
@@ -11514,10 +11691,10 @@
       </c>
     </row>
     <row r="71" spans="2:10">
-      <c r="B71" s="82" t="s">
+      <c r="B71" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="C71" s="82"/>
+      <c r="C71" s="77"/>
       <c r="D71" s="9">
         <v>38</v>
       </c>
@@ -11529,10 +11706,10 @@
       </c>
     </row>
     <row r="72" spans="2:10">
-      <c r="B72" s="82" t="s">
+      <c r="B72" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="82"/>
+      <c r="C72" s="77"/>
       <c r="D72" s="9">
         <v>39</v>
       </c>
@@ -11544,10 +11721,10 @@
       </c>
     </row>
     <row r="73" spans="2:10">
-      <c r="B73" s="82" t="s">
+      <c r="B73" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="82"/>
+      <c r="C73" s="77"/>
       <c r="D73" s="9">
         <v>40</v>
       </c>
@@ -11599,18 +11776,18 @@
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="63" t="s">
+      <c r="B81" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
+      <c r="C81" s="81"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="81"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="63"/>
-      <c r="C82" s="63"/>
-      <c r="D82" s="63"/>
-      <c r="E82" s="63"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="81"/>
+      <c r="D82" s="81"/>
+      <c r="E82" s="81"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="10" t="s">
@@ -11701,18 +11878,18 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="64" t="s">
+      <c r="B97" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="64"/>
-      <c r="D97" s="64"/>
-      <c r="E97" s="64"/>
+      <c r="C97" s="82"/>
+      <c r="D97" s="82"/>
+      <c r="E97" s="82"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="64"/>
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
+      <c r="B98" s="82"/>
+      <c r="C98" s="82"/>
+      <c r="D98" s="82"/>
+      <c r="E98" s="82"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="10" t="s">
@@ -11803,22 +11980,22 @@
       </c>
     </row>
     <row r="114" spans="2:14">
-      <c r="B114" s="65" t="s">
+      <c r="B114" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="65"/>
-      <c r="D114" s="65"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="65"/>
-      <c r="G114" s="65"/>
+      <c r="C114" s="83"/>
+      <c r="D114" s="83"/>
+      <c r="E114" s="83"/>
+      <c r="F114" s="83"/>
+      <c r="G114" s="83"/>
     </row>
     <row r="115" spans="2:14">
-      <c r="B115" s="65"/>
-      <c r="C115" s="65"/>
-      <c r="D115" s="65"/>
-      <c r="E115" s="65"/>
-      <c r="F115" s="65"/>
-      <c r="G115" s="65"/>
+      <c r="B115" s="83"/>
+      <c r="C115" s="83"/>
+      <c r="D115" s="83"/>
+      <c r="E115" s="83"/>
+      <c r="F115" s="83"/>
+      <c r="G115" s="83"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="10" t="s">
@@ -11923,11 +12100,11 @@
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="L120" s="84" t="s">
+      <c r="L120" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="M120" s="85"/>
-      <c r="N120" s="85"/>
+      <c r="M120" s="70"/>
+      <c r="N120" s="70"/>
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="3" t="s">
@@ -11950,9 +12127,9 @@
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="L121" s="85"/>
-      <c r="M121" s="85"/>
-      <c r="N121" s="85"/>
+      <c r="L121" s="70"/>
+      <c r="M121" s="70"/>
+      <c r="N121" s="70"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="3" t="s">
@@ -11975,10 +12152,10 @@
       <c r="D123" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J123" s="83" t="s">
+      <c r="J123" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="K123" s="83"/>
+      <c r="K123" s="68"/>
       <c r="L123" s="21" t="str" cm="1">
         <f t="array" ref="L123:L125">_xlfn.UNIQUE(B118:B127)</f>
         <v>Laptop</v>
@@ -12035,20 +12212,20 @@
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="64" t="s">
+      <c r="B130" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="64"/>
-      <c r="D130" s="64"/>
-      <c r="E130" s="64"/>
-      <c r="F130" s="64"/>
+      <c r="C130" s="82"/>
+      <c r="D130" s="82"/>
+      <c r="E130" s="82"/>
+      <c r="F130" s="82"/>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" s="64"/>
-      <c r="C131" s="64"/>
-      <c r="D131" s="64"/>
-      <c r="E131" s="64"/>
-      <c r="F131" s="64"/>
+      <c r="B131" s="82"/>
+      <c r="C131" s="82"/>
+      <c r="D131" s="82"/>
+      <c r="E131" s="82"/>
+      <c r="F131" s="82"/>
     </row>
     <row r="133" spans="2:11">
       <c r="B133" s="10" t="s">
@@ -12093,10 +12270,10 @@
       <c r="I135" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="J135" s="86" t="s">
+      <c r="J135" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="87"/>
+      <c r="K135" s="72"/>
     </row>
     <row r="136" spans="2:11">
       <c r="B136" s="3" t="s">
@@ -12112,11 +12289,11 @@
       <c r="I136" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J136" s="86">
+      <c r="J136" s="71">
         <f>IFERROR(VLOOKUP($J$135,$B$134:$D$143,2,FALSE),"Not found")</f>
         <v>300</v>
       </c>
-      <c r="K136" s="87"/>
+      <c r="K136" s="72"/>
     </row>
     <row r="137" spans="2:11">
       <c r="B137" s="3" t="s">
@@ -12215,10 +12392,10 @@
       <c r="E146" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="88" t="s">
+      <c r="G146" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="H146" s="89"/>
+      <c r="H146" s="74"/>
     </row>
     <row r="147" spans="2:10" ht="16.8" customHeight="1">
       <c r="B147" s="3" t="s">
@@ -12233,14 +12410,14 @@
       <c r="E147" s="3">
         <v>85</v>
       </c>
-      <c r="G147" s="62" t="s">
+      <c r="G147" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="H147" s="62"/>
-      <c r="I147" s="91" t="s">
+      <c r="H147" s="64"/>
+      <c r="I147" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="J147" s="91"/>
+      <c r="J147" s="66"/>
     </row>
     <row r="148" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B148" s="3" t="s">
@@ -12255,11 +12432,11 @@
       <c r="E148" s="3">
         <v>78</v>
       </c>
-      <c r="I148" s="92" t="str">
+      <c r="I148" s="67" t="str">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,2,FALSE),"NOT FOUND")</f>
         <v>charlie@email.com</v>
       </c>
-      <c r="J148" s="92"/>
+      <c r="J148" s="67"/>
     </row>
     <row r="149" spans="2:10" ht="22.2" customHeight="1">
       <c r="B149" s="3" t="s">
@@ -12274,11 +12451,11 @@
       <c r="E149" s="3">
         <v>92</v>
       </c>
-      <c r="I149" s="92">
+      <c r="I149" s="67">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,3,FALSE),"NOT FOUND")</f>
         <v>7654321098</v>
       </c>
-      <c r="J149" s="92"/>
+      <c r="J149" s="67"/>
     </row>
     <row r="150" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B150" s="3" t="s">
@@ -12293,11 +12470,11 @@
       <c r="E150" s="3">
         <v>67</v>
       </c>
-      <c r="I150" s="92">
+      <c r="I150" s="67">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,4,FALSE),"NOT FOUND")</f>
         <v>92</v>
       </c>
-      <c r="J150" s="92"/>
+      <c r="J150" s="67"/>
     </row>
     <row r="151" spans="2:10" ht="21.6" customHeight="1">
       <c r="B151" s="3" t="s">
@@ -12312,8 +12489,8 @@
       <c r="E151" s="3">
         <v>74</v>
       </c>
-      <c r="I151" s="90"/>
-      <c r="J151" s="90"/>
+      <c r="I151" s="65"/>
+      <c r="J151" s="65"/>
     </row>
     <row r="152" spans="2:10" ht="21.6" customHeight="1"/>
   </sheetData>
@@ -12322,33 +12499,6 @@
     <sortCondition descending="1" ref="C33:C52"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="I151:J151"/>
-    <mergeCell ref="G147:H147"/>
-    <mergeCell ref="I147:J147"/>
-    <mergeCell ref="I148:J148"/>
-    <mergeCell ref="I149:J149"/>
-    <mergeCell ref="I150:J150"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="L120:N121"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G10"/>
     <mergeCell ref="B81:E82"/>
     <mergeCell ref="B97:E98"/>
     <mergeCell ref="B114:G115"/>
@@ -12365,6 +12515,33 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="C61:D61"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G10"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="L120:N121"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="I151:J151"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="I147:J147"/>
+    <mergeCell ref="I148:J148"/>
+    <mergeCell ref="I149:J149"/>
+    <mergeCell ref="I150:J150"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="C8:C27">
@@ -12586,6 +12763,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35914A46-0205-471D-B2D7-66681A3205BE}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:U78"/>
   <sheetViews>
     <sheetView topLeftCell="P44" workbookViewId="0">
@@ -12866,11 +13046,11 @@
       <c r="J38" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="97" t="s">
+      <c r="L38" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="M38" s="97"/>
-      <c r="N38" s="97"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="96"/>
       <c r="R38" s="14" t="s">
         <v>86</v>
       </c>
@@ -12916,9 +13096,9 @@
         <f>IF(AND(G39&gt;70,I39="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L39" s="97"/>
-      <c r="M39" s="97"/>
-      <c r="N39" s="97"/>
+      <c r="L39" s="96"/>
+      <c r="M39" s="96"/>
+      <c r="N39" s="96"/>
       <c r="R39" s="47">
         <v>104</v>
       </c>
@@ -12964,11 +13144,11 @@
         <f t="shared" ref="J40:J58" si="0">IF(AND(G40&gt;70,I40="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L40" s="98" t="s">
+      <c r="L40" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="M40" s="98"/>
-      <c r="N40" s="98"/>
+      <c r="M40" s="95"/>
+      <c r="N40" s="95"/>
       <c r="R40" s="47">
         <v>108</v>
       </c>
@@ -13017,11 +13197,11 @@
       <c r="L41" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="M41" s="98">
+      <c r="M41" s="95">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,2,FALSE),"Not found")</f>
         <v>22</v>
       </c>
-      <c r="N41" s="98"/>
+      <c r="N41" s="95"/>
       <c r="R41" s="47">
         <v>112</v>
       </c>
@@ -13070,11 +13250,11 @@
       <c r="L42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="98" t="str">
+      <c r="M42" s="95" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,3,FALSE),"Not found")</f>
         <v>david@email.com</v>
       </c>
-      <c r="N42" s="98"/>
+      <c r="N42" s="95"/>
       <c r="R42" s="47">
         <v>120</v>
       </c>
@@ -13123,11 +13303,11 @@
       <c r="L43" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="98">
+      <c r="M43" s="95">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,4,FALSE),"Not found")</f>
         <v>6543210987</v>
       </c>
-      <c r="N43" s="98"/>
+      <c r="N43" s="95"/>
       <c r="R43" s="47" t="s">
         <v>87</v>
       </c>
@@ -13176,11 +13356,11 @@
       <c r="L44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M44" s="98">
+      <c r="M44" s="95">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,5,FALSE),"Not found")</f>
         <v>11</v>
       </c>
-      <c r="N44" s="98"/>
+      <c r="N44" s="95"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="37">
@@ -13217,11 +13397,11 @@
       <c r="L45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="98">
+      <c r="M45" s="95">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,6,FALSE),"Not found")</f>
         <v>67</v>
       </c>
-      <c r="N45" s="98"/>
+      <c r="N45" s="95"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="37">
@@ -13258,11 +13438,11 @@
       <c r="L46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="M46" s="98">
+      <c r="M46" s="95">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,7,FALSE),"Not found")</f>
         <v>85</v>
       </c>
-      <c r="N46" s="98"/>
+      <c r="N46" s="95"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="37">
@@ -13299,11 +13479,11 @@
       <c r="L47" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="98" t="str">
+      <c r="M47" s="95" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,8,FALSE),"Not found")</f>
         <v>No</v>
       </c>
-      <c r="N47" s="98"/>
+      <c r="N47" s="95"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="37">
@@ -13337,8 +13517,8 @@
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="M48" s="90"/>
-      <c r="N48" s="90"/>
+      <c r="M48" s="65"/>
+      <c r="N48" s="65"/>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="37">
@@ -13841,10 +14021,10 @@
       <c r="D68" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="94">
+      <c r="F68" s="98">
         <v>103</v>
       </c>
-      <c r="G68" s="94"/>
+      <c r="G68" s="98"/>
       <c r="N68" s="44">
         <v>92</v>
       </c>
@@ -13862,11 +14042,11 @@
       <c r="D69" s="48">
         <v>85</v>
       </c>
-      <c r="F69" s="95" t="str">
+      <c r="F69" s="99" t="str">
         <f>VLOOKUP($F$68,$A$68:$D$71,2,FALSE)</f>
         <v>Charlie</v>
       </c>
-      <c r="G69" s="95"/>
+      <c r="G69" s="99"/>
       <c r="N69" s="44">
         <v>95</v>
       </c>
@@ -13884,11 +14064,11 @@
       <c r="D70" s="48">
         <v>78</v>
       </c>
-      <c r="F70" s="96">
+      <c r="F70" s="100">
         <f>VLOOKUP($F$68,$A$68:$D$71,3,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="G70" s="96"/>
+      <c r="G70" s="100"/>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" s="48">
@@ -13903,27 +14083,27 @@
       <c r="D71" s="48">
         <v>92</v>
       </c>
-      <c r="F71" s="83">
+      <c r="F71" s="68">
         <f>VLOOKUP($F$68,$A$68:$D$71,4,FALSE)</f>
         <v>92</v>
       </c>
-      <c r="G71" s="83"/>
+      <c r="G71" s="68"/>
     </row>
     <row r="74" spans="1:15">
-      <c r="F74" s="93"/>
-      <c r="G74" s="93"/>
+      <c r="F74" s="97"/>
+      <c r="G74" s="97"/>
     </row>
     <row r="75" spans="1:15">
-      <c r="F75" s="93"/>
-      <c r="G75" s="93"/>
+      <c r="F75" s="97"/>
+      <c r="G75" s="97"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="F76" s="93"/>
-      <c r="G76" s="93"/>
+      <c r="F76" s="97"/>
+      <c r="G76" s="97"/>
     </row>
     <row r="77" spans="1:15">
-      <c r="F77" s="93"/>
-      <c r="G77" s="93"/>
+      <c r="F77" s="97"/>
+      <c r="G77" s="97"/>
     </row>
     <row r="78" spans="1:15">
       <c r="F78" s="53"/>
@@ -13936,16 +14116,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="18">
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="L38:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
     <mergeCell ref="F75:G75"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F77:G77"/>
@@ -13954,6 +14124,16 @@
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F74:G74"/>
+    <mergeCell ref="L38:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M48:N48"/>
   </mergeCells>
   <conditionalFormatting sqref="M47:N47">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
@@ -14035,9 +14215,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AF317E-9EAE-490E-A6DA-3381FFA4FB86}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="D4:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="F3" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
@@ -14065,22 +14248,22 @@
     </row>
     <row r="15" spans="4:15">
       <c r="I15" s="56"/>
-      <c r="L15" s="101" t="s">
+      <c r="L15" s="103" t="s">
         <v>205</v>
       </c>
-      <c r="M15" s="102"/>
+      <c r="M15" s="104"/>
       <c r="N15" s="9"/>
       <c r="O15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="4:15">
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="L16" s="98" t="s">
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="L16" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="M16" s="98"/>
+      <c r="M16" s="95"/>
       <c r="N16" s="9"/>
       <c r="O16" t="b">
         <v>1</v>
@@ -14088,26 +14271,26 @@
     </row>
     <row r="17" spans="6:15">
       <c r="I17" s="55"/>
-      <c r="L17" s="98" t="s">
+      <c r="L17" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="M17" s="98"/>
+      <c r="M17" s="95"/>
       <c r="N17" s="9"/>
       <c r="O17" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="6:15">
-      <c r="F18" s="100" t="s">
+      <c r="F18" s="101" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="101"/>
       <c r="I18" s="55"/>
-      <c r="L18" s="98" t="s">
+      <c r="L18" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="M18" s="98"/>
+      <c r="M18" s="95"/>
       <c r="N18" s="9"/>
       <c r="O18" t="b">
         <v>1</v>
@@ -14115,17 +14298,17 @@
     </row>
     <row r="19" spans="6:15">
       <c r="F19" s="38"/>
-      <c r="G19" s="98" t="s">
+      <c r="G19" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="98"/>
+      <c r="H19" s="95"/>
       <c r="I19" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="L19" s="98" t="s">
+      <c r="L19" s="95" t="s">
         <v>209</v>
       </c>
-      <c r="M19" s="98"/>
+      <c r="M19" s="95"/>
       <c r="N19" s="9"/>
       <c r="O19" t="b">
         <v>1</v>
@@ -14133,17 +14316,17 @@
     </row>
     <row r="20" spans="6:15">
       <c r="F20" s="38"/>
-      <c r="G20" s="98" t="s">
+      <c r="G20" s="95" t="s">
         <v>198</v>
       </c>
-      <c r="H20" s="98"/>
+      <c r="H20" s="95"/>
       <c r="I20" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="L20" s="98" t="s">
+      <c r="L20" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="M20" s="98"/>
+      <c r="M20" s="95"/>
       <c r="N20" s="9"/>
       <c r="O20" t="b">
         <v>1</v>
@@ -14151,40 +14334,40 @@
     </row>
     <row r="21" spans="6:15">
       <c r="F21" s="38"/>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="98"/>
+      <c r="H21" s="95"/>
       <c r="I21" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="6:15">
       <c r="F22" s="38"/>
-      <c r="G22" s="98" t="s">
+      <c r="G22" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="98"/>
+      <c r="H22" s="95"/>
       <c r="I22" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="6:15">
       <c r="F23" s="38"/>
-      <c r="G23" s="98" t="s">
+      <c r="G23" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="H23" s="98"/>
+      <c r="H23" s="95"/>
       <c r="I23" s="56" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="6:15">
       <c r="F24" s="38"/>
-      <c r="G24" s="98" t="s">
+      <c r="G24" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="H24" s="98"/>
+      <c r="H24" s="95"/>
       <c r="I24" s="56" t="b">
         <v>0</v>
       </c>
@@ -14198,31 +14381,31 @@
       </c>
     </row>
     <row r="25" spans="6:15">
-      <c r="I25" s="99">
+      <c r="I25" s="102">
         <f>COUNTIF(I19:I24,TRUE)/COUNTA(G19:H24)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J25" s="99"/>
+      <c r="J25" s="102"/>
     </row>
     <row r="26" spans="6:15">
       <c r="I26" s="57">
         <f>1-I25</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="L26" s="103">
+      <c r="L26" s="58">
         <f>M24/L24</f>
         <v>1</v>
       </c>
-      <c r="M26" s="103"/>
-      <c r="N26" s="103"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
     </row>
     <row r="27" spans="6:15">
-      <c r="L27" s="104">
+      <c r="L27" s="59">
         <f>1-L26</f>
         <v>0</v>
       </c>
-      <c r="M27" s="104"/>
-      <c r="N27" s="104"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
     </row>
     <row r="28" spans="6:15">
       <c r="F28" s="55">
@@ -14238,13 +14421,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="L15:M15"/>
@@ -14253,6 +14429,13 @@
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="I25">
@@ -14629,4 +14812,234 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656A5C69-821D-46C1-9FC1-9252AA0BDDC7}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.4">
+      <c r="A1" s="105" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="106" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="107" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="108" t="s">
+        <v>224</v>
+      </c>
+      <c r="F19" s="108"/>
+      <c r="H19" s="110" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="110"/>
+      <c r="N19" s="110"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="3">
+        <v>101</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E20" s="95">
+        <v>101</v>
+      </c>
+      <c r="F20" s="95"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="3">
+        <v>102</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3">
+        <v>60000</v>
+      </c>
+      <c r="E21" s="109">
+        <f>IFERROR(VLOOKUP(E20,A20:C22,3,FALSE), "invalid ID")</f>
+        <v>50000</v>
+      </c>
+      <c r="F21" s="109"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="3">
+        <v>103</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E26" s="108" t="s">
+        <v>230</v>
+      </c>
+      <c r="F26" s="108"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="3">
+        <v>70000</v>
+      </c>
+      <c r="E27" s="95" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="95"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E28" s="109">
+        <f>IFERROR(VLOOKUP(E27,A27:C29,3,FALSE), "Product not found")</f>
+        <v>50000</v>
+      </c>
+      <c r="F28" s="109"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="3">
+        <v>30000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H19:N20"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add desing of the tracking
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D354F7-FB8B-4F44-AB0E-B579F97A1ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D7ABA-0D06-4DF7-A6D4-0795514CF661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="348" windowWidth="17280" windowHeight="9420" firstSheet="3" activeTab="5" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="5" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="273">
   <si>
     <t>Day</t>
   </si>
@@ -1577,19 +1577,25 @@
     <t>completion</t>
   </si>
   <si>
-    <t>person 1</t>
-  </si>
-  <si>
-    <t>person 2</t>
-  </si>
-  <si>
-    <t>person 3</t>
-  </si>
-  <si>
-    <t>person 4</t>
-  </si>
-  <si>
-    <t>person 5</t>
+    <t>Project 1</t>
+  </si>
+  <si>
+    <t>Project 3</t>
+  </si>
+  <si>
+    <t>Project 2</t>
+  </si>
+  <si>
+    <t>Project 4</t>
+  </si>
+  <si>
+    <t>Project 5</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -1600,7 +1606,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1781,6 +1787,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -1886,7 +1899,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1944,86 +1957,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2031,7 +1964,7 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2193,54 +2126,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2255,6 +2140,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2283,11 +2174,47 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2301,7 +2228,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -2313,17 +2243,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2334,15 +2255,25 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -2350,7 +2281,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4740,10 +4678,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4942,19 +4880,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>person 1</c:v>
+                  <c:v>Project 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>person 2</c:v>
+                  <c:v>Project 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>person 3</c:v>
+                  <c:v>Project 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>person 4</c:v>
+                  <c:v>Project 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>person 5</c:v>
+                  <c:v>Project 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4966,16 +4904,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -9693,7 +9631,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9721,7 +9659,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9733,7 +9671,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11525,7 +11463,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>426720</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12396,7 +12334,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>426720</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12463,7 +12401,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>426720</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12530,7 +12468,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>426720</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14232,44 +14170,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -14281,22 +14219,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="86"/>
-      <c r="H7" s="85" t="s">
+      <c r="G7" s="87"/>
+      <c r="H7" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85" t="s">
+      <c r="I7" s="76"/>
+      <c r="J7" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="85"/>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -14309,26 +14247,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="84">
+      <c r="F8" s="77">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84">
+      <c r="G8" s="77"/>
+      <c r="H8" s="77">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84">
+      <c r="I8" s="77"/>
+      <c r="J8" s="77">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84">
+      <c r="K8" s="77"/>
+      <c r="L8" s="77">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="84"/>
+      <c r="M8" s="77"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -14341,14 +14279,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -14361,14 +14299,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -14423,10 +14361,10 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F14" s="94" t="s">
+      <c r="F14" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="94"/>
+      <c r="G14" s="80"/>
       <c r="K14" s="15" t="s">
         <v>66</v>
       </c>
@@ -14609,15 +14547,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="95" t="s">
+      <c r="B30" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="96"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="10" t="s">
@@ -14651,14 +14589,14 @@
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="97" t="s">
+      <c r="F34" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="97"/>
-      <c r="J34" s="97" t="s">
+      <c r="G34" s="83"/>
+      <c r="J34" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="97"/>
+      <c r="K34" s="83"/>
       <c r="M34" s="14" t="s">
         <v>86</v>
       </c>
@@ -14830,10 +14768,10 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="93" t="s">
+      <c r="I42" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="93"/>
+      <c r="J42" s="79"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
@@ -14949,11 +14887,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.6">
-      <c r="B57" s="92" t="s">
+      <c r="B57" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="92"/>
-      <c r="D57" s="92"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="78"/>
       <c r="E57" s="17"/>
       <c r="H57">
         <v>123</v>
@@ -14963,9 +14901,9 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="92"/>
-      <c r="C58" s="92"/>
-      <c r="D58" s="92"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="78"/>
       <c r="E58" s="17"/>
       <c r="H58">
         <v>124</v>
@@ -14983,11 +14921,11 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="98" t="s">
+      <c r="B60" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="98"/>
-      <c r="D60" s="98"/>
+      <c r="C60" s="84"/>
+      <c r="D60" s="84"/>
       <c r="H60">
         <v>126</v>
       </c>
@@ -14999,10 +14937,10 @@
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="99" t="s">
+      <c r="C61" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="100"/>
+      <c r="D61" s="86"/>
       <c r="H61">
         <v>127</v>
       </c>
@@ -15014,10 +14952,10 @@
       <c r="B62" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="81" t="s">
+      <c r="C62" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="82"/>
+      <c r="D62" s="89"/>
       <c r="H62">
         <v>128</v>
       </c>
@@ -15029,10 +14967,10 @@
       <c r="B63" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="81" t="s">
+      <c r="C63" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="82"/>
+      <c r="D63" s="89"/>
       <c r="H63">
         <v>129</v>
       </c>
@@ -15044,10 +14982,10 @@
       <c r="B64" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="81" t="s">
+      <c r="C64" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="82"/>
+      <c r="D64" s="89"/>
       <c r="H64">
         <v>130</v>
       </c>
@@ -15072,10 +15010,10 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="B67" s="83" t="s">
+      <c r="B67" s="90" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="83"/>
+      <c r="C67" s="90"/>
       <c r="D67" s="9">
         <v>34</v>
       </c>
@@ -15087,10 +15025,10 @@
       </c>
     </row>
     <row r="68" spans="2:10">
-      <c r="B68" s="83" t="s">
+      <c r="B68" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="83"/>
+      <c r="C68" s="90"/>
       <c r="D68" s="9">
         <v>35</v>
       </c>
@@ -15102,10 +15040,10 @@
       </c>
     </row>
     <row r="69" spans="2:10">
-      <c r="B69" s="83" t="s">
+      <c r="B69" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="83"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="9">
         <v>36</v>
       </c>
@@ -15120,10 +15058,10 @@
       </c>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="83" t="s">
+      <c r="B70" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="C70" s="83"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="9">
         <v>37</v>
       </c>
@@ -15135,10 +15073,10 @@
       </c>
     </row>
     <row r="71" spans="2:10">
-      <c r="B71" s="83" t="s">
+      <c r="B71" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="C71" s="83"/>
+      <c r="C71" s="90"/>
       <c r="D71" s="9">
         <v>38</v>
       </c>
@@ -15150,10 +15088,10 @@
       </c>
     </row>
     <row r="72" spans="2:10">
-      <c r="B72" s="83" t="s">
+      <c r="B72" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="83"/>
+      <c r="C72" s="90"/>
       <c r="D72" s="9">
         <v>39</v>
       </c>
@@ -15165,10 +15103,10 @@
       </c>
     </row>
     <row r="73" spans="2:10">
-      <c r="B73" s="83" t="s">
+      <c r="B73" s="90" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="83"/>
+      <c r="C73" s="90"/>
       <c r="D73" s="9">
         <v>40</v>
       </c>
@@ -15220,18 +15158,18 @@
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="87" t="s">
+      <c r="B81" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="87"/>
-      <c r="D81" s="87"/>
-      <c r="E81" s="87"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="87"/>
-      <c r="C82" s="87"/>
-      <c r="D82" s="87"/>
-      <c r="E82" s="87"/>
+      <c r="B82" s="71"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="71"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="10" t="s">
@@ -15322,18 +15260,18 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="88" t="s">
+      <c r="B97" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="88"/>
-      <c r="D97" s="88"/>
-      <c r="E97" s="88"/>
+      <c r="C97" s="72"/>
+      <c r="D97" s="72"/>
+      <c r="E97" s="72"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="88"/>
-      <c r="C98" s="88"/>
-      <c r="D98" s="88"/>
-      <c r="E98" s="88"/>
+      <c r="B98" s="72"/>
+      <c r="C98" s="72"/>
+      <c r="D98" s="72"/>
+      <c r="E98" s="72"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="10" t="s">
@@ -15424,22 +15362,22 @@
       </c>
     </row>
     <row r="114" spans="2:14">
-      <c r="B114" s="89" t="s">
+      <c r="B114" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="89"/>
-      <c r="D114" s="89"/>
-      <c r="E114" s="89"/>
-      <c r="F114" s="89"/>
-      <c r="G114" s="89"/>
+      <c r="C114" s="73"/>
+      <c r="D114" s="73"/>
+      <c r="E114" s="73"/>
+      <c r="F114" s="73"/>
+      <c r="G114" s="73"/>
     </row>
     <row r="115" spans="2:14">
-      <c r="B115" s="89"/>
-      <c r="C115" s="89"/>
-      <c r="D115" s="89"/>
-      <c r="E115" s="89"/>
-      <c r="F115" s="89"/>
-      <c r="G115" s="89"/>
+      <c r="B115" s="73"/>
+      <c r="C115" s="73"/>
+      <c r="D115" s="73"/>
+      <c r="E115" s="73"/>
+      <c r="F115" s="73"/>
+      <c r="G115" s="73"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="10" t="s">
@@ -15544,11 +15482,11 @@
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="L120" s="75" t="s">
+      <c r="L120" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="M120" s="76"/>
-      <c r="N120" s="76"/>
+      <c r="M120" s="93"/>
+      <c r="N120" s="93"/>
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="3" t="s">
@@ -15571,9 +15509,9 @@
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="L121" s="76"/>
-      <c r="M121" s="76"/>
-      <c r="N121" s="76"/>
+      <c r="L121" s="93"/>
+      <c r="M121" s="93"/>
+      <c r="N121" s="93"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="3" t="s">
@@ -15596,10 +15534,10 @@
       <c r="D123" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J123" s="74" t="s">
+      <c r="J123" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="K123" s="74"/>
+      <c r="K123" s="91"/>
       <c r="L123" s="21" t="str" cm="1">
         <f t="array" ref="L123:L125">_xlfn.UNIQUE(B118:B127)</f>
         <v>Laptop</v>
@@ -15656,20 +15594,20 @@
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="88" t="s">
+      <c r="B130" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="88"/>
-      <c r="D130" s="88"/>
-      <c r="E130" s="88"/>
-      <c r="F130" s="88"/>
+      <c r="C130" s="72"/>
+      <c r="D130" s="72"/>
+      <c r="E130" s="72"/>
+      <c r="F130" s="72"/>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" s="88"/>
-      <c r="C131" s="88"/>
-      <c r="D131" s="88"/>
-      <c r="E131" s="88"/>
-      <c r="F131" s="88"/>
+      <c r="B131" s="72"/>
+      <c r="C131" s="72"/>
+      <c r="D131" s="72"/>
+      <c r="E131" s="72"/>
+      <c r="F131" s="72"/>
     </row>
     <row r="133" spans="2:11">
       <c r="B133" s="10" t="s">
@@ -15714,10 +15652,10 @@
       <c r="I135" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="J135" s="77" t="s">
+      <c r="J135" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="78"/>
+      <c r="K135" s="95"/>
     </row>
     <row r="136" spans="2:11">
       <c r="B136" s="3" t="s">
@@ -15733,11 +15671,11 @@
       <c r="I136" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J136" s="77">
+      <c r="J136" s="94">
         <f>IFERROR(VLOOKUP($J$135,$B$134:$D$143,2,FALSE),"Not found")</f>
         <v>300</v>
       </c>
-      <c r="K136" s="78"/>
+      <c r="K136" s="95"/>
     </row>
     <row r="137" spans="2:11">
       <c r="B137" s="3" t="s">
@@ -15836,10 +15774,10 @@
       <c r="E146" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="79" t="s">
+      <c r="G146" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="H146" s="80"/>
+      <c r="H146" s="97"/>
     </row>
     <row r="147" spans="2:10" ht="16.8" customHeight="1">
       <c r="B147" s="3" t="s">
@@ -15858,10 +15796,10 @@
         <v>135</v>
       </c>
       <c r="H147" s="70"/>
-      <c r="I147" s="72" t="s">
+      <c r="I147" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="J147" s="72"/>
+      <c r="J147" s="99"/>
     </row>
     <row r="148" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B148" s="3" t="s">
@@ -15876,11 +15814,11 @@
       <c r="E148" s="3">
         <v>78</v>
       </c>
-      <c r="I148" s="73" t="str">
+      <c r="I148" s="100" t="str">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,2,FALSE),"NOT FOUND")</f>
         <v>charlie@email.com</v>
       </c>
-      <c r="J148" s="73"/>
+      <c r="J148" s="100"/>
     </row>
     <row r="149" spans="2:10" ht="22.2" customHeight="1">
       <c r="B149" s="3" t="s">
@@ -15895,11 +15833,11 @@
       <c r="E149" s="3">
         <v>92</v>
       </c>
-      <c r="I149" s="73">
+      <c r="I149" s="100">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,3,FALSE),"NOT FOUND")</f>
         <v>7654321098</v>
       </c>
-      <c r="J149" s="73"/>
+      <c r="J149" s="100"/>
     </row>
     <row r="150" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B150" s="3" t="s">
@@ -15914,11 +15852,11 @@
       <c r="E150" s="3">
         <v>67</v>
       </c>
-      <c r="I150" s="73">
+      <c r="I150" s="100">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,4,FALSE),"NOT FOUND")</f>
         <v>92</v>
       </c>
-      <c r="J150" s="73"/>
+      <c r="J150" s="100"/>
     </row>
     <row r="151" spans="2:10" ht="21.6" customHeight="1">
       <c r="B151" s="3" t="s">
@@ -15933,8 +15871,8 @@
       <c r="E151" s="3">
         <v>74</v>
       </c>
-      <c r="I151" s="71"/>
-      <c r="J151" s="71"/>
+      <c r="I151" s="98"/>
+      <c r="J151" s="98"/>
     </row>
     <row r="152" spans="2:10" ht="21.6" customHeight="1"/>
   </sheetData>
@@ -15943,6 +15881,33 @@
     <sortCondition descending="1" ref="C33:C52"/>
   </sortState>
   <mergeCells count="43">
+    <mergeCell ref="I151:J151"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="I147:J147"/>
+    <mergeCell ref="I148:J148"/>
+    <mergeCell ref="I149:J149"/>
+    <mergeCell ref="I150:J150"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="L120:N121"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G10"/>
     <mergeCell ref="B81:E82"/>
     <mergeCell ref="B97:E98"/>
     <mergeCell ref="B114:G115"/>
@@ -15959,42 +15924,15 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="C61:D61"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G10"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="L120:N121"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="I151:J151"/>
-    <mergeCell ref="G147:H147"/>
-    <mergeCell ref="I147:J147"/>
-    <mergeCell ref="I148:J148"/>
-    <mergeCell ref="I149:J149"/>
-    <mergeCell ref="I150:J150"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="C8:C27">
-    <cfRule type="cellIs" dxfId="19" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="31" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D27">
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThan">
       <formula>"PASS"</formula>
     </cfRule>
     <cfRule type="iconSet" priority="29">
@@ -16006,10 +15944,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:D73">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>37</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="between">
       <formula>34</formula>
       <formula>38</formula>
     </cfRule>
@@ -16070,18 +16008,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:C95">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:C110">
-    <cfRule type="top10" dxfId="14" priority="17" rank="5"/>
+    <cfRule type="top10" dxfId="15" priority="17" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C134:C143">
-    <cfRule type="top10" dxfId="13" priority="5" rank="5"/>
+    <cfRule type="top10" dxfId="14" priority="5" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>AND(C134&gt;500,D134="North")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16490,11 +16428,11 @@
       <c r="J38" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="102" t="s">
+      <c r="L38" s="105" t="s">
         <v>187</v>
       </c>
-      <c r="M38" s="102"/>
-      <c r="N38" s="102"/>
+      <c r="M38" s="105"/>
+      <c r="N38" s="105"/>
       <c r="R38" s="14" t="s">
         <v>86</v>
       </c>
@@ -16540,9 +16478,9 @@
         <f>IF(AND(G39&gt;70,I39="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L39" s="102"/>
-      <c r="M39" s="102"/>
-      <c r="N39" s="102"/>
+      <c r="L39" s="105"/>
+      <c r="M39" s="105"/>
+      <c r="N39" s="105"/>
       <c r="R39" s="47">
         <v>104</v>
       </c>
@@ -16588,11 +16526,11 @@
         <f t="shared" ref="J40:J58" si="0">IF(AND(G40&gt;70,I40="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L40" s="101" t="s">
+      <c r="L40" s="106" t="s">
         <v>194</v>
       </c>
-      <c r="M40" s="101"/>
-      <c r="N40" s="101"/>
+      <c r="M40" s="106"/>
+      <c r="N40" s="106"/>
       <c r="R40" s="47">
         <v>108</v>
       </c>
@@ -16641,11 +16579,11 @@
       <c r="L41" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="M41" s="101">
+      <c r="M41" s="106">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,2,FALSE),"Not found")</f>
         <v>22</v>
       </c>
-      <c r="N41" s="101"/>
+      <c r="N41" s="106"/>
       <c r="R41" s="47">
         <v>112</v>
       </c>
@@ -16694,11 +16632,11 @@
       <c r="L42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="101" t="str">
+      <c r="M42" s="106" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,3,FALSE),"Not found")</f>
         <v>david@email.com</v>
       </c>
-      <c r="N42" s="101"/>
+      <c r="N42" s="106"/>
       <c r="R42" s="47">
         <v>120</v>
       </c>
@@ -16747,11 +16685,11 @@
       <c r="L43" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="101">
+      <c r="M43" s="106">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,4,FALSE),"Not found")</f>
         <v>6543210987</v>
       </c>
-      <c r="N43" s="101"/>
+      <c r="N43" s="106"/>
       <c r="R43" s="47" t="s">
         <v>87</v>
       </c>
@@ -16800,11 +16738,11 @@
       <c r="L44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M44" s="101">
+      <c r="M44" s="106">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,5,FALSE),"Not found")</f>
         <v>11</v>
       </c>
-      <c r="N44" s="101"/>
+      <c r="N44" s="106"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="37">
@@ -16841,11 +16779,11 @@
       <c r="L45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="101">
+      <c r="M45" s="106">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,6,FALSE),"Not found")</f>
         <v>67</v>
       </c>
-      <c r="N45" s="101"/>
+      <c r="N45" s="106"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="37">
@@ -16882,11 +16820,11 @@
       <c r="L46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="M46" s="101">
+      <c r="M46" s="106">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,7,FALSE),"Not found")</f>
         <v>85</v>
       </c>
-      <c r="N46" s="101"/>
+      <c r="N46" s="106"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="37">
@@ -16923,11 +16861,11 @@
       <c r="L47" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="101" t="str">
+      <c r="M47" s="106" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,8,FALSE),"Not found")</f>
         <v>No</v>
       </c>
-      <c r="N47" s="101"/>
+      <c r="N47" s="106"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="37">
@@ -16961,8 +16899,8 @@
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="M48" s="71"/>
-      <c r="N48" s="71"/>
+      <c r="M48" s="98"/>
+      <c r="N48" s="98"/>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="37">
@@ -17465,10 +17403,10 @@
       <c r="D68" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="104">
+      <c r="F68" s="102">
         <v>103</v>
       </c>
-      <c r="G68" s="104"/>
+      <c r="G68" s="102"/>
       <c r="N68" s="44">
         <v>92</v>
       </c>
@@ -17486,11 +17424,11 @@
       <c r="D69" s="48">
         <v>85</v>
       </c>
-      <c r="F69" s="105" t="str">
+      <c r="F69" s="103" t="str">
         <f>VLOOKUP($F$68,$A$68:$D$71,2,FALSE)</f>
         <v>Charlie</v>
       </c>
-      <c r="G69" s="105"/>
+      <c r="G69" s="103"/>
       <c r="N69" s="44">
         <v>95</v>
       </c>
@@ -17508,11 +17446,11 @@
       <c r="D70" s="48">
         <v>78</v>
       </c>
-      <c r="F70" s="106">
+      <c r="F70" s="104">
         <f>VLOOKUP($F$68,$A$68:$D$71,3,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="G70" s="106"/>
+      <c r="G70" s="104"/>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" s="48">
@@ -17527,27 +17465,27 @@
       <c r="D71" s="48">
         <v>92</v>
       </c>
-      <c r="F71" s="74">
+      <c r="F71" s="91">
         <f>VLOOKUP($F$68,$A$68:$D$71,4,FALSE)</f>
         <v>92</v>
       </c>
-      <c r="G71" s="74"/>
+      <c r="G71" s="91"/>
     </row>
     <row r="74" spans="1:15">
-      <c r="F74" s="103"/>
-      <c r="G74" s="103"/>
+      <c r="F74" s="101"/>
+      <c r="G74" s="101"/>
     </row>
     <row r="75" spans="1:15">
-      <c r="F75" s="103"/>
-      <c r="G75" s="103"/>
+      <c r="F75" s="101"/>
+      <c r="G75" s="101"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="F76" s="103"/>
-      <c r="G76" s="103"/>
+      <c r="F76" s="101"/>
+      <c r="G76" s="101"/>
     </row>
     <row r="77" spans="1:15">
-      <c r="F77" s="103"/>
-      <c r="G77" s="103"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="101"/>
     </row>
     <row r="78" spans="1:15">
       <c r="F78" s="53"/>
@@ -17560,6 +17498,16 @@
     </sortState>
   </autoFilter>
   <mergeCells count="18">
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="L38:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
     <mergeCell ref="F75:G75"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F77:G77"/>
@@ -17568,32 +17516,22 @@
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F74:G74"/>
-    <mergeCell ref="L38:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="M48:N48"/>
   </mergeCells>
   <conditionalFormatting sqref="M47:N47">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:N46">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I58">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",I39)))</formula>
     </cfRule>
     <cfRule type="iconSet" priority="6">
@@ -17692,22 +17630,22 @@
     </row>
     <row r="15" spans="4:15">
       <c r="I15" s="56"/>
-      <c r="L15" s="109" t="s">
+      <c r="L15" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="M15" s="110"/>
+      <c r="M15" s="109"/>
       <c r="N15" s="9"/>
       <c r="O15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:15">
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="L16" s="101" t="s">
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="L16" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="M16" s="101"/>
+      <c r="M16" s="106"/>
       <c r="N16" s="9"/>
       <c r="O16" t="b">
         <v>1</v>
@@ -17715,26 +17653,26 @@
     </row>
     <row r="17" spans="6:15">
       <c r="I17" s="55"/>
-      <c r="L17" s="101" t="s">
+      <c r="L17" s="106" t="s">
         <v>207</v>
       </c>
-      <c r="M17" s="101"/>
+      <c r="M17" s="106"/>
       <c r="N17" s="9"/>
       <c r="O17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="6:15">
-      <c r="F18" s="107" t="s">
+      <c r="F18" s="110" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
       <c r="I18" s="55"/>
-      <c r="L18" s="101" t="s">
+      <c r="L18" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="M18" s="101"/>
+      <c r="M18" s="106"/>
       <c r="N18" s="9"/>
       <c r="O18" t="b">
         <v>0</v>
@@ -17742,17 +17680,17 @@
     </row>
     <row r="19" spans="6:15">
       <c r="F19" s="38"/>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="101"/>
+      <c r="H19" s="106"/>
       <c r="I19" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="101" t="s">
+      <c r="L19" s="106" t="s">
         <v>209</v>
       </c>
-      <c r="M19" s="101"/>
+      <c r="M19" s="106"/>
       <c r="N19" s="9"/>
       <c r="O19" t="b">
         <v>0</v>
@@ -17760,17 +17698,17 @@
     </row>
     <row r="20" spans="6:15">
       <c r="F20" s="38"/>
-      <c r="G20" s="101" t="s">
+      <c r="G20" s="106" t="s">
         <v>198</v>
       </c>
-      <c r="H20" s="101"/>
+      <c r="H20" s="106"/>
       <c r="I20" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="101" t="s">
+      <c r="L20" s="106" t="s">
         <v>210</v>
       </c>
-      <c r="M20" s="101"/>
+      <c r="M20" s="106"/>
       <c r="N20" s="9"/>
       <c r="O20" t="b">
         <v>1</v>
@@ -17778,40 +17716,40 @@
     </row>
     <row r="21" spans="6:15">
       <c r="F21" s="38"/>
-      <c r="G21" s="101" t="s">
+      <c r="G21" s="106" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="101"/>
+      <c r="H21" s="106"/>
       <c r="I21" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="6:15">
       <c r="F22" s="38"/>
-      <c r="G22" s="101" t="s">
+      <c r="G22" s="106" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="101"/>
+      <c r="H22" s="106"/>
       <c r="I22" s="56" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="6:15">
       <c r="F23" s="38"/>
-      <c r="G23" s="101" t="s">
+      <c r="G23" s="106" t="s">
         <v>201</v>
       </c>
-      <c r="H23" s="101"/>
+      <c r="H23" s="106"/>
       <c r="I23" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="6:15">
       <c r="F24" s="38"/>
-      <c r="G24" s="101" t="s">
+      <c r="G24" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="H24" s="101"/>
+      <c r="H24" s="106"/>
       <c r="I24" s="56" t="b">
         <v>0</v>
       </c>
@@ -17825,11 +17763,11 @@
       </c>
     </row>
     <row r="25" spans="6:15">
-      <c r="I25" s="108">
+      <c r="I25" s="107">
         <f>COUNTIF(I19:I24,TRUE)/COUNTA(G19:H24)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J25" s="108"/>
+      <c r="J25" s="107"/>
     </row>
     <row r="26" spans="6:15">
       <c r="I26" s="57">
@@ -17865,6 +17803,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="L15:M15"/>
@@ -17873,13 +17818,6 @@
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="I25">
@@ -17911,10 +17849,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:M20">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$O15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>$O$15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18321,15 +18259,15 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="114"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -18351,19 +18289,19 @@
       <c r="C19" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E19" s="115" t="s">
+      <c r="E19" s="111" t="s">
         <v>224</v>
       </c>
-      <c r="F19" s="115"/>
-      <c r="H19" s="117" t="s">
+      <c r="F19" s="111"/>
+      <c r="H19" s="113" t="s">
         <v>231</v>
       </c>
-      <c r="I19" s="117"/>
-      <c r="J19" s="117"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
-      <c r="N19" s="117"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
+      <c r="N19" s="113"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="3">
@@ -18375,17 +18313,17 @@
       <c r="C20" s="3">
         <v>50000</v>
       </c>
-      <c r="E20" s="101">
+      <c r="E20" s="106">
         <v>101</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
-      <c r="N20" s="117"/>
+      <c r="F20" s="106"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="113"/>
+      <c r="N20" s="113"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="3">
@@ -18397,11 +18335,11 @@
       <c r="C21" s="3">
         <v>60000</v>
       </c>
-      <c r="E21" s="114">
+      <c r="E21" s="115">
         <f>IFERROR(VLOOKUP(E20,A20:C22,3,FALSE), "invalid ID")</f>
         <v>50000</v>
       </c>
-      <c r="F21" s="114"/>
+      <c r="F21" s="115"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="3">
@@ -18413,11 +18351,11 @@
       <c r="C22" s="3">
         <v>70000</v>
       </c>
-      <c r="H22" s="116" t="s">
+      <c r="H22" s="112" t="s">
         <v>232</v>
       </c>
-      <c r="I22" s="104"/>
-      <c r="J22" s="104"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="26" t="s">
@@ -18434,10 +18372,10 @@
       <c r="C26" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E26" s="115" t="s">
+      <c r="E26" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="F26" s="115"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="3" t="s">
@@ -18449,10 +18387,10 @@
       <c r="C27" s="3">
         <v>70000</v>
       </c>
-      <c r="E27" s="101" t="s">
+      <c r="E27" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="F27" s="101"/>
+      <c r="F27" s="106"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="3" t="s">
@@ -18464,11 +18402,11 @@
       <c r="C28" s="3">
         <v>50000</v>
       </c>
-      <c r="E28" s="114">
+      <c r="E28" s="115">
         <f>IFERROR(VLOOKUP(E27,A27:C29,3,FALSE), "Product not found")</f>
         <v>30000</v>
       </c>
-      <c r="F28" s="114"/>
+      <c r="F28" s="115"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="3" t="s">
@@ -18527,14 +18465,14 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="111" t="s">
+      <c r="A48" s="116" t="s">
         <v>238</v>
       </c>
-      <c r="B48" s="111"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="111"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="116"/>
+      <c r="F48" s="116"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
@@ -18542,13 +18480,13 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="112" t="s">
+      <c r="A51" s="117" t="s">
         <v>239</v>
       </c>
-      <c r="B51" s="112"/>
-      <c r="C51" s="112"/>
-      <c r="D51" s="112"/>
-      <c r="E51" s="112"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="117"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="117"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="10" t="s">
@@ -18690,14 +18628,14 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="113" t="s">
+      <c r="A77" s="114" t="s">
         <v>256</v>
       </c>
-      <c r="B77" s="113"/>
-      <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
-      <c r="E77" s="113"/>
-      <c r="F77" s="113"/>
+      <c r="B77" s="114"/>
+      <c r="C77" s="114"/>
+      <c r="D77" s="114"/>
+      <c r="E77" s="114"/>
+      <c r="F77" s="114"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
@@ -18705,13 +18643,13 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="112" t="s">
+      <c r="A80" s="117" t="s">
         <v>257</v>
       </c>
-      <c r="B80" s="112"/>
-      <c r="C80" s="112"/>
-      <c r="D80" s="112"/>
-      <c r="E80" s="112"/>
+      <c r="B80" s="117"/>
+      <c r="C80" s="117"/>
+      <c r="D80" s="117"/>
+      <c r="E80" s="117"/>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="10" t="s">
@@ -18831,6 +18769,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="H22:J22"/>
@@ -18839,11 +18782,6 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A77:F77"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H22" r:id="rId1" xr:uid="{A99D977A-63CD-4EBC-97DD-2EDD7A39ABBD}"/>
@@ -18858,164 +18796,198 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B25:G33"/>
+  <dimension ref="B24:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="25" spans="2:7" ht="15" thickBot="1"/>
-    <row r="26" spans="2:7">
-      <c r="B26" s="118"/>
-      <c r="C26" s="119" t="s">
+    <row r="24" spans="2:8">
+      <c r="E24" s="119" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="118" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="9"/>
+      <c r="C26" s="120" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="120" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="120" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="119" t="s">
+      <c r="F26" s="120" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="120" t="s">
+      <c r="G26" s="121" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="121" t="s">
+      <c r="H26" s="120" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="122" t="s">
         <v>266</v>
       </c>
-      <c r="C27" s="122" t="b">
+      <c r="C27" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="122" t="b">
+      <c r="D27" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="122" t="b">
+      <c r="E27" s="123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="122" t="b">
+      <c r="G27" s="124">
+        <f>COUNTIF(C27:F27,TRUE)/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="H27" s="9" t="str">
+        <f>IF(G27=1,$E$24,$F$24)</f>
+        <v>In Progress</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="122" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="123">
-        <f>COUNTIF(C27:F27,TRUE)/4</f>
+      <c r="D28" s="123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="121" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="122" t="b">
+      <c r="E28" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="122" t="b">
+      <c r="F28" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="123">
+      <c r="G28" s="124">
         <f t="shared" ref="G28:G31" si="0">COUNTIF(C28:F28,TRUE)/4</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="121" t="s">
-        <v>268</v>
-      </c>
-      <c r="C29" s="122" t="b">
+      <c r="H28" s="9" t="str">
+        <f t="shared" ref="H28:H31" si="1">IF(G28=1,$E$24,$F$24)</f>
+        <v>Completed</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="122" t="b">
+      <c r="D29" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="E29" s="122" t="b">
+      <c r="E29" s="123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="122" t="b">
+      <c r="G29" s="124">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="H29" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>In Progress</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="122" t="s">
+        <v>269</v>
+      </c>
+      <c r="C30" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="123">
+      <c r="D30" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="124">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="H30" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>In Progress</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="122" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="124">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="121" t="s">
-        <v>269</v>
-      </c>
-      <c r="C30" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="122" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="123">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="15" thickBot="1">
-      <c r="B31" s="124" t="s">
-        <v>270</v>
-      </c>
-      <c r="C31" s="125" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" s="125" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="125" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="125" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="126">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7">
+      <c r="H31" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Completed</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
       <c r="G32" s="64">
         <f>SUM(G27:G31)/COUNT(G27:G31)</f>
-        <v>1</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="33" spans="7:7">
       <c r="G33" s="65">
         <f>1-G32</f>
-        <v>0</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="G27:G31">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="5Rating">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="20"/>
-        <cfvo type="percent" val="40"/>
-        <cfvo type="percent" val="60"/>
-        <cfvo type="percent" val="80"/>
-      </iconSet>
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{52A8C0EE-2A05-424A-BB60-9A04D6C3159A}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19128,7 +19100,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>426720</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -19414,7 +19386,7 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>426720</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -19436,7 +19408,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>426720</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -19458,7 +19430,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>426720</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -19468,5 +19440,40 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{52A8C0EE-2A05-424A-BB60-9A04D6C3159A}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G27:G31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{9E849A72-7427-4357-AB85-EAE4E6AB7BFF}">
+            <xm:f>NOT(ISERROR(SEARCH($E$24,H27)))</xm:f>
+            <xm:f>$E$24</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H27:H31</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LEARNE REGRESSION ON EXCEL
</commit_message>
<xml_diff>
--- a/time line.xlsx
+++ b/time line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D7ABA-0D06-4DF7-A6D4-0795514CF661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0291F922-20E1-4A0B-AE3A-8DC5D67BFB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="5" xr2:uid="{86D8B116-CEF7-4802-BD43-6E1B6BD688CB}"/>
   </bookViews>
@@ -2111,6 +2111,13 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2126,6 +2133,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2140,12 +2195,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2174,47 +2223,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2228,10 +2241,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -2243,8 +2253,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2255,25 +2274,6 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -4678,10 +4678,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15000000000000002</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4907,16 +4907,16 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9611,11 +9611,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9643,7 +9643,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9651,15 +9651,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9667,7 +9667,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9675,7 +9675,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9683,7 +9683,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14030,13 +14030,13 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="1:10" ht="60.6" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -14124,14 +14124,14 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="69" t="s">
+      <c r="B9" s="75"/>
+      <c r="C9" s="76" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="70"/>
+      <c r="D9" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -14170,44 +14170,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
     </row>
     <row r="7" spans="1:13" ht="24">
       <c r="B7" s="6" t="s">
@@ -14219,22 +14219,22 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="87"/>
-      <c r="H7" s="76" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76" t="s">
+      <c r="K7" s="92"/>
+      <c r="L7" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="76"/>
+      <c r="M7" s="92"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
@@ -14247,26 +14247,26 @@
         <f>IF(C8&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="91">
         <f>COUNT(C8:C27)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77">
+      <c r="G8" s="91"/>
+      <c r="H8" s="91">
         <f>AVERAGE(C8:C27)</f>
         <v>69.3</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77">
+      <c r="I8" s="91"/>
+      <c r="J8" s="91">
         <f>COUNTIF(D8:D27,"PASS")</f>
         <v>16</v>
       </c>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77">
+      <c r="K8" s="91"/>
+      <c r="L8" s="91">
         <f>F8-J8</f>
         <v>4</v>
       </c>
-      <c r="M8" s="77"/>
+      <c r="M8" s="91"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
@@ -14279,14 +14279,14 @@
         <f t="shared" ref="D9:D27" si="0">IF(C9&gt;=50,$F$15, $G$15)</f>
         <v>PASS</v>
       </c>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="3" t="s">
@@ -14299,14 +14299,14 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="3" t="s">
@@ -14361,10 +14361,10 @@
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="F14" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="80"/>
+      <c r="G14" s="101"/>
       <c r="K14" s="15" t="s">
         <v>66</v>
       </c>
@@ -14547,15 +14547,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="82"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="103"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="10" t="s">
@@ -14589,14 +14589,14 @@
       <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="83" t="s">
+      <c r="F34" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="83"/>
-      <c r="J34" s="83" t="s">
+      <c r="G34" s="104"/>
+      <c r="J34" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="83"/>
+      <c r="K34" s="104"/>
       <c r="M34" s="14" t="s">
         <v>86</v>
       </c>
@@ -14768,10 +14768,10 @@
       <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="79" t="s">
+      <c r="I42" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="79"/>
+      <c r="J42" s="100"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="3" t="s">
@@ -14887,11 +14887,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.6">
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="78"/>
-      <c r="D57" s="78"/>
+      <c r="C57" s="99"/>
+      <c r="D57" s="99"/>
       <c r="E57" s="17"/>
       <c r="H57">
         <v>123</v>
@@ -14901,9 +14901,9 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="78"/>
-      <c r="C58" s="78"/>
-      <c r="D58" s="78"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="99"/>
+      <c r="D58" s="99"/>
       <c r="E58" s="17"/>
       <c r="H58">
         <v>124</v>
@@ -14921,11 +14921,11 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="84" t="s">
+      <c r="B60" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="84"/>
-      <c r="D60" s="84"/>
+      <c r="C60" s="105"/>
+      <c r="D60" s="105"/>
       <c r="H60">
         <v>126</v>
       </c>
@@ -14937,10 +14937,10 @@
       <c r="B61" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="85" t="s">
+      <c r="C61" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="86"/>
+      <c r="D61" s="107"/>
       <c r="H61">
         <v>127</v>
       </c>
@@ -15158,18 +15158,18 @@
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="71" t="s">
+      <c r="B81" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="71"/>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71"/>
+      <c r="C81" s="94"/>
+      <c r="D81" s="94"/>
+      <c r="E81" s="94"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="71"/>
-      <c r="C82" s="71"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
+      <c r="B82" s="94"/>
+      <c r="C82" s="94"/>
+      <c r="D82" s="94"/>
+      <c r="E82" s="94"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="10" t="s">
@@ -15260,18 +15260,18 @@
       </c>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="72" t="s">
+      <c r="B97" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="72"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="72"/>
+      <c r="C97" s="95"/>
+      <c r="D97" s="95"/>
+      <c r="E97" s="95"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="72"/>
-      <c r="C98" s="72"/>
-      <c r="D98" s="72"/>
-      <c r="E98" s="72"/>
+      <c r="B98" s="95"/>
+      <c r="C98" s="95"/>
+      <c r="D98" s="95"/>
+      <c r="E98" s="95"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="10" t="s">
@@ -15362,22 +15362,22 @@
       </c>
     </row>
     <row r="114" spans="2:14">
-      <c r="B114" s="73" t="s">
+      <c r="B114" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="73"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="73"/>
-      <c r="F114" s="73"/>
-      <c r="G114" s="73"/>
+      <c r="C114" s="96"/>
+      <c r="D114" s="96"/>
+      <c r="E114" s="96"/>
+      <c r="F114" s="96"/>
+      <c r="G114" s="96"/>
     </row>
     <row r="115" spans="2:14">
-      <c r="B115" s="73"/>
-      <c r="C115" s="73"/>
-      <c r="D115" s="73"/>
-      <c r="E115" s="73"/>
-      <c r="F115" s="73"/>
-      <c r="G115" s="73"/>
+      <c r="B115" s="96"/>
+      <c r="C115" s="96"/>
+      <c r="D115" s="96"/>
+      <c r="E115" s="96"/>
+      <c r="F115" s="96"/>
+      <c r="G115" s="96"/>
     </row>
     <row r="117" spans="2:14">
       <c r="B117" s="10" t="s">
@@ -15482,11 +15482,11 @@
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="L120" s="92" t="s">
+      <c r="L120" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="M120" s="93"/>
-      <c r="N120" s="93"/>
+      <c r="M120" s="83"/>
+      <c r="N120" s="83"/>
     </row>
     <row r="121" spans="2:14">
       <c r="B121" s="3" t="s">
@@ -15509,9 +15509,9 @@
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="L121" s="93"/>
-      <c r="M121" s="93"/>
-      <c r="N121" s="93"/>
+      <c r="L121" s="83"/>
+      <c r="M121" s="83"/>
+      <c r="N121" s="83"/>
     </row>
     <row r="122" spans="2:14">
       <c r="B122" s="3" t="s">
@@ -15534,10 +15534,10 @@
       <c r="D123" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J123" s="91" t="s">
+      <c r="J123" s="81" t="s">
         <v>120</v>
       </c>
-      <c r="K123" s="91"/>
+      <c r="K123" s="81"/>
       <c r="L123" s="21" t="str" cm="1">
         <f t="array" ref="L123:L125">_xlfn.UNIQUE(B118:B127)</f>
         <v>Laptop</v>
@@ -15594,20 +15594,20 @@
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="72" t="s">
+      <c r="B130" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="72"/>
-      <c r="D130" s="72"/>
-      <c r="E130" s="72"/>
-      <c r="F130" s="72"/>
+      <c r="C130" s="95"/>
+      <c r="D130" s="95"/>
+      <c r="E130" s="95"/>
+      <c r="F130" s="95"/>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" s="72"/>
-      <c r="C131" s="72"/>
-      <c r="D131" s="72"/>
-      <c r="E131" s="72"/>
-      <c r="F131" s="72"/>
+      <c r="B131" s="95"/>
+      <c r="C131" s="95"/>
+      <c r="D131" s="95"/>
+      <c r="E131" s="95"/>
+      <c r="F131" s="95"/>
     </row>
     <row r="133" spans="2:11">
       <c r="B133" s="10" t="s">
@@ -15652,10 +15652,10 @@
       <c r="I135" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="J135" s="94" t="s">
+      <c r="J135" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="95"/>
+      <c r="K135" s="85"/>
     </row>
     <row r="136" spans="2:11">
       <c r="B136" s="3" t="s">
@@ -15671,11 +15671,11 @@
       <c r="I136" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J136" s="94">
+      <c r="J136" s="84">
         <f>IFERROR(VLOOKUP($J$135,$B$134:$D$143,2,FALSE),"Not found")</f>
         <v>300</v>
       </c>
-      <c r="K136" s="95"/>
+      <c r="K136" s="85"/>
     </row>
     <row r="137" spans="2:11">
       <c r="B137" s="3" t="s">
@@ -15774,10 +15774,10 @@
       <c r="E146" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="96" t="s">
+      <c r="G146" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="H146" s="97"/>
+      <c r="H146" s="87"/>
     </row>
     <row r="147" spans="2:10" ht="16.8" customHeight="1">
       <c r="B147" s="3" t="s">
@@ -15792,14 +15792,14 @@
       <c r="E147" s="3">
         <v>85</v>
       </c>
-      <c r="G147" s="70" t="s">
+      <c r="G147" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="H147" s="70"/>
-      <c r="I147" s="99" t="s">
+      <c r="H147" s="77"/>
+      <c r="I147" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="J147" s="99"/>
+      <c r="J147" s="79"/>
     </row>
     <row r="148" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B148" s="3" t="s">
@@ -15814,11 +15814,11 @@
       <c r="E148" s="3">
         <v>78</v>
       </c>
-      <c r="I148" s="100" t="str">
+      <c r="I148" s="80" t="str">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,2,FALSE),"NOT FOUND")</f>
         <v>charlie@email.com</v>
       </c>
-      <c r="J148" s="100"/>
+      <c r="J148" s="80"/>
     </row>
     <row r="149" spans="2:10" ht="22.2" customHeight="1">
       <c r="B149" s="3" t="s">
@@ -15833,11 +15833,11 @@
       <c r="E149" s="3">
         <v>92</v>
       </c>
-      <c r="I149" s="100">
+      <c r="I149" s="80">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,3,FALSE),"NOT FOUND")</f>
         <v>7654321098</v>
       </c>
-      <c r="J149" s="100"/>
+      <c r="J149" s="80"/>
     </row>
     <row r="150" spans="2:10" ht="20.399999999999999" customHeight="1">
       <c r="B150" s="3" t="s">
@@ -15852,11 +15852,11 @@
       <c r="E150" s="3">
         <v>67</v>
       </c>
-      <c r="I150" s="100">
+      <c r="I150" s="80">
         <f>IFERROR(VLOOKUP($I$147,$B$147:$E$151,4,FALSE),"NOT FOUND")</f>
         <v>92</v>
       </c>
-      <c r="J150" s="100"/>
+      <c r="J150" s="80"/>
     </row>
     <row r="151" spans="2:10" ht="21.6" customHeight="1">
       <c r="B151" s="3" t="s">
@@ -15871,8 +15871,8 @@
       <c r="E151" s="3">
         <v>74</v>
       </c>
-      <c r="I151" s="98"/>
-      <c r="J151" s="98"/>
+      <c r="I151" s="78"/>
+      <c r="J151" s="78"/>
     </row>
     <row r="152" spans="2:10" ht="21.6" customHeight="1"/>
   </sheetData>
@@ -15881,33 +15881,6 @@
     <sortCondition descending="1" ref="C33:C52"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="I151:J151"/>
-    <mergeCell ref="G147:H147"/>
-    <mergeCell ref="I147:J147"/>
-    <mergeCell ref="I148:J148"/>
-    <mergeCell ref="I149:J149"/>
-    <mergeCell ref="I150:J150"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="L120:N121"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G10"/>
     <mergeCell ref="B81:E82"/>
     <mergeCell ref="B97:E98"/>
     <mergeCell ref="B114:G115"/>
@@ -15924,6 +15897,33 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="C61:D61"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G10"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="L120:N121"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="I151:J151"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="I147:J147"/>
+    <mergeCell ref="I148:J148"/>
+    <mergeCell ref="I149:J149"/>
+    <mergeCell ref="I150:J150"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="C8:C27">
@@ -16428,11 +16428,11 @@
       <c r="J38" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="105" t="s">
+      <c r="L38" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="M38" s="105"/>
-      <c r="N38" s="105"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
       <c r="R38" s="14" t="s">
         <v>86</v>
       </c>
@@ -16478,9 +16478,9 @@
         <f>IF(AND(G39&gt;70,I39="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L39" s="105"/>
-      <c r="M39" s="105"/>
-      <c r="N39" s="105"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
+      <c r="N39" s="109"/>
       <c r="R39" s="47">
         <v>104</v>
       </c>
@@ -16526,11 +16526,11 @@
         <f t="shared" ref="J40:J58" si="0">IF(AND(G40&gt;70,I40="YES"),"Pass","pending")</f>
         <v>pending</v>
       </c>
-      <c r="L40" s="106" t="s">
+      <c r="L40" s="108" t="s">
         <v>194</v>
       </c>
-      <c r="M40" s="106"/>
-      <c r="N40" s="106"/>
+      <c r="M40" s="108"/>
+      <c r="N40" s="108"/>
       <c r="R40" s="47">
         <v>108</v>
       </c>
@@ -16579,11 +16579,11 @@
       <c r="L41" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="M41" s="106">
+      <c r="M41" s="108">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,2,FALSE),"Not found")</f>
         <v>22</v>
       </c>
-      <c r="N41" s="106"/>
+      <c r="N41" s="108"/>
       <c r="R41" s="47">
         <v>112</v>
       </c>
@@ -16632,11 +16632,11 @@
       <c r="L42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="106" t="str">
+      <c r="M42" s="108" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,3,FALSE),"Not found")</f>
         <v>david@email.com</v>
       </c>
-      <c r="N42" s="106"/>
+      <c r="N42" s="108"/>
       <c r="R42" s="47">
         <v>120</v>
       </c>
@@ -16685,11 +16685,11 @@
       <c r="L43" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="106">
+      <c r="M43" s="108">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,4,FALSE),"Not found")</f>
         <v>6543210987</v>
       </c>
-      <c r="N43" s="106"/>
+      <c r="N43" s="108"/>
       <c r="R43" s="47" t="s">
         <v>87</v>
       </c>
@@ -16738,11 +16738,11 @@
       <c r="L44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="M44" s="106">
+      <c r="M44" s="108">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,5,FALSE),"Not found")</f>
         <v>11</v>
       </c>
-      <c r="N44" s="106"/>
+      <c r="N44" s="108"/>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="37">
@@ -16779,11 +16779,11 @@
       <c r="L45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="106">
+      <c r="M45" s="108">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,6,FALSE),"Not found")</f>
         <v>67</v>
       </c>
-      <c r="N45" s="106"/>
+      <c r="N45" s="108"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="37">
@@ -16820,11 +16820,11 @@
       <c r="L46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="M46" s="106">
+      <c r="M46" s="108">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,7,FALSE),"Not found")</f>
         <v>85</v>
       </c>
-      <c r="N46" s="106"/>
+      <c r="N46" s="108"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="37">
@@ -16861,11 +16861,11 @@
       <c r="L47" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="106" t="str">
+      <c r="M47" s="108" t="str">
         <f>IFERROR(VLOOKUP($L$40,$B$39:$I$58,8,FALSE),"Not found")</f>
         <v>No</v>
       </c>
-      <c r="N47" s="106"/>
+      <c r="N47" s="108"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="37">
@@ -16899,8 +16899,8 @@
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
-      <c r="M48" s="98"/>
-      <c r="N48" s="98"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="78"/>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="37">
@@ -17403,10 +17403,10 @@
       <c r="D68" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="102">
+      <c r="F68" s="111">
         <v>103</v>
       </c>
-      <c r="G68" s="102"/>
+      <c r="G68" s="111"/>
       <c r="N68" s="44">
         <v>92</v>
       </c>
@@ -17424,11 +17424,11 @@
       <c r="D69" s="48">
         <v>85</v>
       </c>
-      <c r="F69" s="103" t="str">
+      <c r="F69" s="112" t="str">
         <f>VLOOKUP($F$68,$A$68:$D$71,2,FALSE)</f>
         <v>Charlie</v>
       </c>
-      <c r="G69" s="103"/>
+      <c r="G69" s="112"/>
       <c r="N69" s="44">
         <v>95</v>
       </c>
@@ -17446,11 +17446,11 @@
       <c r="D70" s="48">
         <v>78</v>
       </c>
-      <c r="F70" s="104">
+      <c r="F70" s="113">
         <f>VLOOKUP($F$68,$A$68:$D$71,3,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="G70" s="104"/>
+      <c r="G70" s="113"/>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" s="48">
@@ -17465,27 +17465,27 @@
       <c r="D71" s="48">
         <v>92</v>
       </c>
-      <c r="F71" s="91">
+      <c r="F71" s="81">
         <f>VLOOKUP($F$68,$A$68:$D$71,4,FALSE)</f>
         <v>92</v>
       </c>
-      <c r="G71" s="91"/>
+      <c r="G71" s="81"/>
     </row>
     <row r="74" spans="1:15">
-      <c r="F74" s="101"/>
-      <c r="G74" s="101"/>
+      <c r="F74" s="110"/>
+      <c r="G74" s="110"/>
     </row>
     <row r="75" spans="1:15">
-      <c r="F75" s="101"/>
-      <c r="G75" s="101"/>
+      <c r="F75" s="110"/>
+      <c r="G75" s="110"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="F76" s="101"/>
-      <c r="G76" s="101"/>
+      <c r="F76" s="110"/>
+      <c r="G76" s="110"/>
     </row>
     <row r="77" spans="1:15">
-      <c r="F77" s="101"/>
-      <c r="G77" s="101"/>
+      <c r="F77" s="110"/>
+      <c r="G77" s="110"/>
     </row>
     <row r="78" spans="1:15">
       <c r="F78" s="53"/>
@@ -17498,16 +17498,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="18">
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="L38:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
     <mergeCell ref="F75:G75"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F77:G77"/>
@@ -17516,6 +17506,16 @@
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F74:G74"/>
+    <mergeCell ref="L38:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M48:N48"/>
   </mergeCells>
   <conditionalFormatting sqref="M47:N47">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
@@ -17630,22 +17630,22 @@
     </row>
     <row r="15" spans="4:15">
       <c r="I15" s="56"/>
-      <c r="L15" s="108" t="s">
+      <c r="L15" s="116" t="s">
         <v>205</v>
       </c>
-      <c r="M15" s="109"/>
+      <c r="M15" s="117"/>
       <c r="N15" s="9"/>
       <c r="O15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:15">
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="L16" s="106" t="s">
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="L16" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="M16" s="106"/>
+      <c r="M16" s="108"/>
       <c r="N16" s="9"/>
       <c r="O16" t="b">
         <v>1</v>
@@ -17653,26 +17653,26 @@
     </row>
     <row r="17" spans="6:15">
       <c r="I17" s="55"/>
-      <c r="L17" s="106" t="s">
+      <c r="L17" s="108" t="s">
         <v>207</v>
       </c>
-      <c r="M17" s="106"/>
+      <c r="M17" s="108"/>
       <c r="N17" s="9"/>
       <c r="O17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="6:15">
-      <c r="F18" s="110" t="s">
+      <c r="F18" s="114" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
       <c r="I18" s="55"/>
-      <c r="L18" s="106" t="s">
+      <c r="L18" s="108" t="s">
         <v>208</v>
       </c>
-      <c r="M18" s="106"/>
+      <c r="M18" s="108"/>
       <c r="N18" s="9"/>
       <c r="O18" t="b">
         <v>0</v>
@@ -17680,17 +17680,17 @@
     </row>
     <row r="19" spans="6:15">
       <c r="F19" s="38"/>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="108" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="106"/>
+      <c r="H19" s="108"/>
       <c r="I19" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="106" t="s">
+      <c r="L19" s="108" t="s">
         <v>209</v>
       </c>
-      <c r="M19" s="106"/>
+      <c r="M19" s="108"/>
       <c r="N19" s="9"/>
       <c r="O19" t="b">
         <v>0</v>
@@ -17698,17 +17698,17 @@
     </row>
     <row r="20" spans="6:15">
       <c r="F20" s="38"/>
-      <c r="G20" s="106" t="s">
+      <c r="G20" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="H20" s="106"/>
+      <c r="H20" s="108"/>
       <c r="I20" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="106" t="s">
+      <c r="L20" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="M20" s="106"/>
+      <c r="M20" s="108"/>
       <c r="N20" s="9"/>
       <c r="O20" t="b">
         <v>1</v>
@@ -17716,40 +17716,40 @@
     </row>
     <row r="21" spans="6:15">
       <c r="F21" s="38"/>
-      <c r="G21" s="106" t="s">
+      <c r="G21" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="106"/>
+      <c r="H21" s="108"/>
       <c r="I21" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="6:15">
       <c r="F22" s="38"/>
-      <c r="G22" s="106" t="s">
+      <c r="G22" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="106"/>
+      <c r="H22" s="108"/>
       <c r="I22" s="56" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="6:15">
       <c r="F23" s="38"/>
-      <c r="G23" s="106" t="s">
+      <c r="G23" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="H23" s="106"/>
+      <c r="H23" s="108"/>
       <c r="I23" s="56" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="6:15">
       <c r="F24" s="38"/>
-      <c r="G24" s="106" t="s">
+      <c r="G24" s="108" t="s">
         <v>202</v>
       </c>
-      <c r="H24" s="106"/>
+      <c r="H24" s="108"/>
       <c r="I24" s="56" t="b">
         <v>0</v>
       </c>
@@ -17763,11 +17763,11 @@
       </c>
     </row>
     <row r="25" spans="6:15">
-      <c r="I25" s="107">
+      <c r="I25" s="115">
         <f>COUNTIF(I19:I24,TRUE)/COUNTA(G19:H24)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J25" s="107"/>
+      <c r="J25" s="115"/>
     </row>
     <row r="26" spans="6:15">
       <c r="I26" s="57">
@@ -17803,13 +17803,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="L15:M15"/>
@@ -17818,6 +17811,13 @@
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="I25">
@@ -18259,15 +18259,15 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="114"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -18289,19 +18289,19 @@
       <c r="C19" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E19" s="111" t="s">
+      <c r="E19" s="122" t="s">
         <v>224</v>
       </c>
-      <c r="F19" s="111"/>
-      <c r="H19" s="113" t="s">
+      <c r="F19" s="122"/>
+      <c r="H19" s="124" t="s">
         <v>231</v>
       </c>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="113"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="124"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="3">
@@ -18313,17 +18313,17 @@
       <c r="C20" s="3">
         <v>50000</v>
       </c>
-      <c r="E20" s="106">
+      <c r="E20" s="108">
         <v>101</v>
       </c>
-      <c r="F20" s="106"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
-      <c r="M20" s="113"/>
-      <c r="N20" s="113"/>
+      <c r="F20" s="108"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="124"/>
+      <c r="K20" s="124"/>
+      <c r="L20" s="124"/>
+      <c r="M20" s="124"/>
+      <c r="N20" s="124"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="3">
@@ -18335,11 +18335,11 @@
       <c r="C21" s="3">
         <v>60000</v>
       </c>
-      <c r="E21" s="115">
+      <c r="E21" s="121">
         <f>IFERROR(VLOOKUP(E20,A20:C22,3,FALSE), "invalid ID")</f>
         <v>50000</v>
       </c>
-      <c r="F21" s="115"/>
+      <c r="F21" s="121"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="3">
@@ -18351,11 +18351,11 @@
       <c r="C22" s="3">
         <v>70000</v>
       </c>
-      <c r="H22" s="112" t="s">
+      <c r="H22" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="26" t="s">
@@ -18372,10 +18372,10 @@
       <c r="C26" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E26" s="111" t="s">
+      <c r="E26" s="122" t="s">
         <v>230</v>
       </c>
-      <c r="F26" s="111"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="3" t="s">
@@ -18387,10 +18387,10 @@
       <c r="C27" s="3">
         <v>70000</v>
       </c>
-      <c r="E27" s="106" t="s">
+      <c r="E27" s="108" t="s">
         <v>247</v>
       </c>
-      <c r="F27" s="106"/>
+      <c r="F27" s="108"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="3" t="s">
@@ -18402,11 +18402,11 @@
       <c r="C28" s="3">
         <v>50000</v>
       </c>
-      <c r="E28" s="115">
+      <c r="E28" s="121">
         <f>IFERROR(VLOOKUP(E27,A27:C29,3,FALSE), "Product not found")</f>
         <v>30000</v>
       </c>
-      <c r="F28" s="115"/>
+      <c r="F28" s="121"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="3" t="s">
@@ -18465,14 +18465,14 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="116"/>
-      <c r="E48" s="116"/>
-      <c r="F48" s="116"/>
+      <c r="B48" s="118"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="118"/>
+      <c r="F48" s="118"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
@@ -18480,13 +18480,13 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="117" t="s">
+      <c r="A51" s="119" t="s">
         <v>239</v>
       </c>
-      <c r="B51" s="117"/>
-      <c r="C51" s="117"/>
-      <c r="D51" s="117"/>
-      <c r="E51" s="117"/>
+      <c r="B51" s="119"/>
+      <c r="C51" s="119"/>
+      <c r="D51" s="119"/>
+      <c r="E51" s="119"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="10" t="s">
@@ -18628,14 +18628,14 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="114" t="s">
+      <c r="A77" s="120" t="s">
         <v>256</v>
       </c>
-      <c r="B77" s="114"/>
-      <c r="C77" s="114"/>
-      <c r="D77" s="114"/>
-      <c r="E77" s="114"/>
-      <c r="F77" s="114"/>
+      <c r="B77" s="120"/>
+      <c r="C77" s="120"/>
+      <c r="D77" s="120"/>
+      <c r="E77" s="120"/>
+      <c r="F77" s="120"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
@@ -18643,13 +18643,13 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="117" t="s">
+      <c r="A80" s="119" t="s">
         <v>257</v>
       </c>
-      <c r="B80" s="117"/>
-      <c r="C80" s="117"/>
-      <c r="D80" s="117"/>
-      <c r="E80" s="117"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="119"/>
+      <c r="D80" s="119"/>
+      <c r="E80" s="119"/>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="10" t="s">
@@ -18769,11 +18769,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A77:F77"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="E28:F28"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="H22:J22"/>
@@ -18782,6 +18777,11 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H22" r:id="rId1" xr:uid="{A99D977A-63CD-4EBC-97DD-2EDD7A39ABBD}"/>
@@ -18798,7 +18798,7 @@
   </sheetPr>
   <dimension ref="B24:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -18809,51 +18809,51 @@
   </cols>
   <sheetData>
     <row r="24" spans="2:8">
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="67" t="s">
         <v>271</v>
       </c>
-      <c r="F24" s="118" t="s">
+      <c r="F24" s="66" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="9"/>
-      <c r="C26" s="120" t="s">
+      <c r="C26" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="120" t="s">
+      <c r="D26" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="120" t="s">
+      <c r="E26" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="120" t="s">
+      <c r="F26" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="121" t="s">
+      <c r="G26" s="69" t="s">
         <v>265</v>
       </c>
-      <c r="H26" s="120" t="s">
+      <c r="H26" s="68" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="C27" s="123" t="b">
+      <c r="C27" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="123" t="b">
+      <c r="D27" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="123" t="b">
+      <c r="E27" s="71" t="b">
         <v>0</v>
       </c>
-      <c r="F27" s="123" t="b">
+      <c r="F27" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="124">
+      <c r="G27" s="72">
         <f>COUNTIF(C27:F27,TRUE)/4</f>
         <v>0.75</v>
       </c>
@@ -18863,49 +18863,49 @@
       </c>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="70" t="s">
         <v>268</v>
       </c>
-      <c r="C28" s="123" t="b">
+      <c r="C28" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="124">
+      <c r="F28" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="72">
         <f t="shared" ref="G28:G31" si="0">COUNTIF(C28:F28,TRUE)/4</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="H28" s="9" t="str">
         <f t="shared" ref="H28:H31" si="1">IF(G28=1,$E$24,$F$24)</f>
-        <v>Completed</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="122" t="s">
+      <c r="B29" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="C29" s="123" t="b">
+      <c r="C29" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="123" t="b">
+      <c r="F29" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="E29" s="123" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="124">
+      <c r="G29" s="72">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H29" s="9" t="str">
         <f t="shared" si="1"/>
@@ -18913,24 +18913,24 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="122" t="s">
+      <c r="B30" s="70" t="s">
         <v>269</v>
       </c>
-      <c r="C30" s="123" t="b">
+      <c r="C30" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="D30" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="123" t="b">
+      <c r="D30" s="71" t="b">
         <v>0</v>
       </c>
-      <c r="F30" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="124">
+      <c r="E30" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="72">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="H30" s="9" t="str">
         <f t="shared" si="1"/>
@@ -18938,40 +18938,40 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="122" t="s">
+      <c r="B31" s="70" t="s">
         <v>270</v>
       </c>
-      <c r="C31" s="123" t="b">
+      <c r="C31" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="D31" s="123" t="b">
+      <c r="D31" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="E31" s="123" t="b">
+      <c r="F31" s="71" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="123" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="124">
+      <c r="G31" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H31" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>Completed</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="G32" s="64">
         <f>SUM(G27:G31)/COUNT(G27:G31)</f>
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="7:7">
       <c r="G33" s="65">
         <f>1-G32</f>
-        <v>0.15000000000000002</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>